<commit_message>
Chromaticity Diagrams for Laboratory Results Calculated. Missing: online results
</commit_message>
<xml_diff>
--- a/Documents/Color Mixtures/Color Blends.xlsx
+++ b/Documents/Color Mixtures/Color Blends.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PauloGarcia/Desktop/blendingbox/Color Mixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PauloGarcia/Desktop/blendingbox/Documents/Color Mixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Color Mixtures First Study" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="264">
   <si>
     <t>Cores a Misturar</t>
   </si>
@@ -812,6 +812,12 @@
   </si>
   <si>
     <t>lapso</t>
+  </si>
+  <si>
+    <t>Perguntas com cores semelhantes:</t>
+  </si>
+  <si>
+    <t>#5 + #8 + #16</t>
   </si>
 </sst>
 </file>
@@ -2055,7 +2061,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="405">
+  <cellXfs count="407">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2936,7 +2942,73 @@
     <xf numFmtId="0" fontId="0" fillId="117" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="43" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="42" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="41" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2945,7 +3017,31 @@
     <xf numFmtId="2" fontId="0" fillId="41" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="41" borderId="37" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="41" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2954,34 +3050,85 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="41" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2996,229 +3143,94 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="41" borderId="37" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="43" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="42" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3616,10 +3628,10 @@
   </sheetPr>
   <dimension ref="A2:AI60"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A5" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="X27" sqref="X27"/>
+      <selection pane="topRight" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3634,10 +3646,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B2" s="330" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="330"/>
+      <c r="B2" s="364" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="364"/>
       <c r="E2" t="s">
         <v>7</v>
       </c>
@@ -3820,10 +3832,10 @@
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B10" s="335" t="s">
+      <c r="B10" s="368" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="335"/>
+      <c r="C10" s="368"/>
       <c r="D10" s="4">
         <v>0</v>
       </c>
@@ -3878,10 +3890,10 @@
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B11" s="336" t="s">
+      <c r="B11" s="369" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="336"/>
+      <c r="C11" s="369"/>
       <c r="D11" s="4">
         <v>120</v>
       </c>
@@ -3936,10 +3948,10 @@
       </c>
     </row>
     <row r="12" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="337" t="s">
+      <c r="B12" s="370" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="337"/>
+      <c r="C12" s="370"/>
       <c r="D12" s="25">
         <v>240</v>
       </c>
@@ -3994,10 +4006,10 @@
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B13" s="338" t="s">
+      <c r="B13" s="371" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="338"/>
+      <c r="C13" s="371"/>
       <c r="D13" s="4">
         <v>180</v>
       </c>
@@ -4052,10 +4064,10 @@
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B14" s="339" t="s">
+      <c r="B14" s="372" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="339"/>
+      <c r="C14" s="372"/>
       <c r="D14" s="4">
         <v>300</v>
       </c>
@@ -4110,10 +4122,10 @@
       </c>
     </row>
     <row r="15" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="334" t="s">
+      <c r="B15" s="367" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="334"/>
+      <c r="C15" s="367"/>
       <c r="D15" s="6">
         <v>60</v>
       </c>
@@ -4169,52 +4181,52 @@
     </row>
     <row r="16" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:35" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="355" t="s">
+      <c r="B17" s="336" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="356"/>
-      <c r="D17" s="331" t="s">
+      <c r="C17" s="337"/>
+      <c r="D17" s="350" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="332"/>
-      <c r="F17" s="333"/>
-      <c r="G17" s="332" t="s">
+      <c r="E17" s="329"/>
+      <c r="F17" s="330"/>
+      <c r="G17" s="329" t="s">
         <v>9</v>
       </c>
-      <c r="H17" s="332"/>
-      <c r="I17" s="333"/>
-      <c r="J17" s="331" t="s">
+      <c r="H17" s="329"/>
+      <c r="I17" s="330"/>
+      <c r="J17" s="350" t="s">
         <v>10</v>
       </c>
-      <c r="K17" s="332"/>
-      <c r="L17" s="332"/>
-      <c r="M17" s="333"/>
-      <c r="N17" s="331" t="s">
+      <c r="K17" s="329"/>
+      <c r="L17" s="329"/>
+      <c r="M17" s="330"/>
+      <c r="N17" s="350" t="s">
         <v>27</v>
       </c>
-      <c r="O17" s="332"/>
-      <c r="P17" s="332"/>
-      <c r="Q17" s="347" t="s">
+      <c r="O17" s="329"/>
+      <c r="P17" s="329"/>
+      <c r="Q17" s="351" t="s">
         <v>91</v>
       </c>
-      <c r="R17" s="348"/>
-      <c r="S17" s="349"/>
-      <c r="T17" s="344" t="s">
+      <c r="R17" s="352"/>
+      <c r="S17" s="353"/>
+      <c r="T17" s="346" t="s">
         <v>51</v>
       </c>
-      <c r="U17" s="345"/>
-      <c r="V17" s="345"/>
-      <c r="W17" s="345"/>
-      <c r="X17" s="345"/>
-      <c r="Y17" s="345"/>
-      <c r="Z17" s="345"/>
-      <c r="AA17" s="345"/>
-      <c r="AB17" s="345"/>
-      <c r="AC17" s="346"/>
+      <c r="U17" s="347"/>
+      <c r="V17" s="347"/>
+      <c r="W17" s="347"/>
+      <c r="X17" s="347"/>
+      <c r="Y17" s="347"/>
+      <c r="Z17" s="347"/>
+      <c r="AA17" s="347"/>
+      <c r="AB17" s="347"/>
+      <c r="AC17" s="348"/>
     </row>
     <row r="18" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="357"/>
-      <c r="C18" s="358"/>
+      <c r="B18" s="338"/>
+      <c r="C18" s="339"/>
       <c r="D18" s="22" t="s">
         <v>37</v>
       </c>
@@ -4263,32 +4275,32 @@
       <c r="S18" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="T18" s="350" t="s">
+      <c r="T18" s="354" t="s">
         <v>8</v>
       </c>
-      <c r="U18" s="351"/>
-      <c r="V18" s="352" t="s">
+      <c r="U18" s="355"/>
+      <c r="V18" s="356" t="s">
         <v>92</v>
       </c>
-      <c r="W18" s="351"/>
-      <c r="X18" s="352" t="s">
+      <c r="W18" s="355"/>
+      <c r="X18" s="356" t="s">
         <v>10</v>
       </c>
-      <c r="Y18" s="351"/>
-      <c r="Z18" s="352" t="s">
+      <c r="Y18" s="355"/>
+      <c r="Z18" s="356" t="s">
         <v>27</v>
       </c>
-      <c r="AA18" s="351"/>
-      <c r="AB18" s="353" t="s">
+      <c r="AA18" s="355"/>
+      <c r="AB18" s="357" t="s">
         <v>91</v>
       </c>
-      <c r="AC18" s="354"/>
+      <c r="AC18" s="358"/>
     </row>
     <row r="19" spans="1:35" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="361" t="s">
+      <c r="B19" s="342" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="362"/>
+      <c r="C19" s="343"/>
       <c r="D19" s="20">
         <v>60</v>
       </c>
@@ -4362,15 +4374,15 @@
         <v>94</v>
       </c>
       <c r="AC19" s="75"/>
-      <c r="AD19" s="341" t="s">
+      <c r="AD19" s="349" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B20" s="361" t="s">
+      <c r="B20" s="342" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="362"/>
+      <c r="C20" s="343"/>
       <c r="D20" s="20">
         <v>300</v>
       </c>
@@ -4444,13 +4456,13 @@
         <v>95</v>
       </c>
       <c r="AC20" s="76"/>
-      <c r="AD20" s="341"/>
+      <c r="AD20" s="349"/>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B21" s="314" t="s">
+      <c r="B21" s="344" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="315"/>
+      <c r="C21" s="345"/>
       <c r="D21" s="20">
         <v>180</v>
       </c>
@@ -4525,16 +4537,16 @@
         <v>96</v>
       </c>
       <c r="AC21" s="80"/>
-      <c r="AD21" s="341"/>
+      <c r="AD21" s="349"/>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A22" s="310" t="s">
+      <c r="A22" s="381" t="s">
         <v>116</v>
       </c>
-      <c r="B22" s="316" t="s">
+      <c r="B22" s="361" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="317"/>
+      <c r="C22" s="362"/>
       <c r="D22" s="94">
         <v>90</v>
       </c>
@@ -4609,12 +4621,12 @@
         <v>97</v>
       </c>
       <c r="AC22" s="104"/>
-      <c r="AD22" s="341"/>
+      <c r="AD22" s="349"/>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A23" s="310"/>
-      <c r="B23" s="318"/>
-      <c r="C23" s="319"/>
+      <c r="A23" s="381"/>
+      <c r="B23" s="365"/>
+      <c r="C23" s="366"/>
       <c r="D23" s="105">
         <v>270</v>
       </c>
@@ -4624,38 +4636,38 @@
       <c r="F23" s="107">
         <v>100</v>
       </c>
-      <c r="G23" s="311"/>
-      <c r="H23" s="312"/>
-      <c r="I23" s="313"/>
-      <c r="J23" s="320"/>
-      <c r="K23" s="321"/>
-      <c r="L23" s="321"/>
-      <c r="M23" s="322"/>
-      <c r="N23" s="320"/>
-      <c r="O23" s="321"/>
-      <c r="P23" s="322"/>
-      <c r="Q23" s="311"/>
-      <c r="R23" s="312"/>
-      <c r="S23" s="323"/>
+      <c r="G23" s="333"/>
+      <c r="H23" s="334"/>
+      <c r="I23" s="380"/>
+      <c r="J23" s="331"/>
+      <c r="K23" s="379"/>
+      <c r="L23" s="379"/>
+      <c r="M23" s="332"/>
+      <c r="N23" s="331"/>
+      <c r="O23" s="379"/>
+      <c r="P23" s="332"/>
+      <c r="Q23" s="333"/>
+      <c r="R23" s="334"/>
+      <c r="S23" s="335"/>
       <c r="T23" s="302" t="s">
         <v>114</v>
       </c>
       <c r="U23" s="109"/>
-      <c r="V23" s="320"/>
-      <c r="W23" s="322"/>
-      <c r="X23" s="320"/>
-      <c r="Y23" s="322"/>
-      <c r="Z23" s="320"/>
-      <c r="AA23" s="322"/>
-      <c r="AB23" s="320"/>
-      <c r="AC23" s="322"/>
-      <c r="AD23" s="341"/>
+      <c r="V23" s="331"/>
+      <c r="W23" s="332"/>
+      <c r="X23" s="331"/>
+      <c r="Y23" s="332"/>
+      <c r="Z23" s="331"/>
+      <c r="AA23" s="332"/>
+      <c r="AB23" s="331"/>
+      <c r="AC23" s="332"/>
+      <c r="AD23" s="349"/>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B24" s="314" t="s">
+      <c r="B24" s="344" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="315"/>
+      <c r="C24" s="345"/>
       <c r="D24" s="20">
         <v>330</v>
       </c>
@@ -4729,13 +4741,13 @@
         <v>98</v>
       </c>
       <c r="AC24" s="81"/>
-      <c r="AD24" s="341"/>
+      <c r="AD24" s="349"/>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B25" s="314" t="s">
+      <c r="B25" s="344" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="315"/>
+      <c r="C25" s="345"/>
       <c r="D25" s="20">
         <v>30</v>
       </c>
@@ -4810,13 +4822,13 @@
         <v>99</v>
       </c>
       <c r="AC25" s="82"/>
-      <c r="AD25" s="341"/>
+      <c r="AD25" s="349"/>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B26" s="314" t="s">
+      <c r="B26" s="344" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="315"/>
+      <c r="C26" s="345"/>
       <c r="D26" s="20">
         <v>240</v>
       </c>
@@ -4891,13 +4903,13 @@
         <v>100</v>
       </c>
       <c r="AC26" s="83"/>
-      <c r="AD26" s="341"/>
+      <c r="AD26" s="349"/>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B27" s="314" t="s">
+      <c r="B27" s="344" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="315"/>
+      <c r="C27" s="345"/>
       <c r="D27" s="20">
         <v>0</v>
       </c>
@@ -4971,13 +4983,13 @@
         <v>101</v>
       </c>
       <c r="AC27" s="84"/>
-      <c r="AD27" s="341"/>
+      <c r="AD27" s="349"/>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B28" s="314" t="s">
+      <c r="B28" s="344" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="315"/>
+      <c r="C28" s="345"/>
       <c r="D28" s="20">
         <v>150</v>
       </c>
@@ -5052,16 +5064,16 @@
         <v>102</v>
       </c>
       <c r="AC28" s="85"/>
-      <c r="AD28" s="341"/>
+      <c r="AD28" s="349"/>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A29" s="310" t="s">
+      <c r="A29" s="381" t="s">
         <v>116</v>
       </c>
-      <c r="B29" s="316" t="s">
+      <c r="B29" s="361" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="317"/>
+      <c r="C29" s="362"/>
       <c r="D29" s="94">
         <v>210</v>
       </c>
@@ -5135,12 +5147,12 @@
         <v>103</v>
       </c>
       <c r="AC29" s="111"/>
-      <c r="AD29" s="341"/>
+      <c r="AD29" s="349"/>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A30" s="310"/>
-      <c r="B30" s="318"/>
-      <c r="C30" s="319"/>
+      <c r="A30" s="381"/>
+      <c r="B30" s="365"/>
+      <c r="C30" s="366"/>
       <c r="D30" s="105">
         <v>30</v>
       </c>
@@ -5150,38 +5162,38 @@
       <c r="F30" s="107">
         <v>100</v>
       </c>
-      <c r="G30" s="311"/>
-      <c r="H30" s="312"/>
-      <c r="I30" s="313"/>
-      <c r="J30" s="320"/>
-      <c r="K30" s="321"/>
-      <c r="L30" s="321"/>
-      <c r="M30" s="322"/>
-      <c r="N30" s="320"/>
-      <c r="O30" s="321"/>
-      <c r="P30" s="322"/>
-      <c r="Q30" s="311"/>
-      <c r="R30" s="312"/>
-      <c r="S30" s="323"/>
+      <c r="G30" s="333"/>
+      <c r="H30" s="334"/>
+      <c r="I30" s="380"/>
+      <c r="J30" s="331"/>
+      <c r="K30" s="379"/>
+      <c r="L30" s="379"/>
+      <c r="M30" s="332"/>
+      <c r="N30" s="331"/>
+      <c r="O30" s="379"/>
+      <c r="P30" s="332"/>
+      <c r="Q30" s="333"/>
+      <c r="R30" s="334"/>
+      <c r="S30" s="335"/>
       <c r="T30" s="302" t="s">
         <v>115</v>
       </c>
       <c r="U30" s="112"/>
-      <c r="V30" s="320"/>
-      <c r="W30" s="322"/>
-      <c r="X30" s="320"/>
-      <c r="Y30" s="322"/>
-      <c r="Z30" s="320"/>
-      <c r="AA30" s="322"/>
-      <c r="AB30" s="320"/>
-      <c r="AC30" s="322"/>
-      <c r="AD30" s="341"/>
+      <c r="V30" s="331"/>
+      <c r="W30" s="332"/>
+      <c r="X30" s="331"/>
+      <c r="Y30" s="332"/>
+      <c r="Z30" s="331"/>
+      <c r="AA30" s="332"/>
+      <c r="AB30" s="331"/>
+      <c r="AC30" s="332"/>
+      <c r="AD30" s="349"/>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B31" s="314" t="s">
+      <c r="B31" s="344" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="315"/>
+      <c r="C31" s="345"/>
       <c r="D31" s="20">
         <v>90</v>
       </c>
@@ -5256,17 +5268,17 @@
         <v>104</v>
       </c>
       <c r="AC31" s="86"/>
-      <c r="AD31" s="341"/>
-      <c r="AH31" s="330" t="s">
+      <c r="AD31" s="349"/>
+      <c r="AH31" s="364" t="s">
         <v>93</v>
       </c>
-      <c r="AI31" s="330"/>
+      <c r="AI31" s="364"/>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B32" s="314" t="s">
+      <c r="B32" s="344" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="315"/>
+      <c r="C32" s="345"/>
       <c r="D32" s="20">
         <v>210</v>
       </c>
@@ -5341,13 +5353,13 @@
         <v>105</v>
       </c>
       <c r="AC32" s="87"/>
-      <c r="AD32" s="341"/>
+      <c r="AD32" s="349"/>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B33" s="314" t="s">
+      <c r="B33" s="344" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="315"/>
+      <c r="C33" s="345"/>
       <c r="D33" s="20">
         <v>270</v>
       </c>
@@ -5422,16 +5434,16 @@
         <v>106</v>
       </c>
       <c r="AC33" s="88"/>
-      <c r="AD33" s="341"/>
+      <c r="AD33" s="349"/>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A34" s="310" t="s">
+      <c r="A34" s="381" t="s">
         <v>116</v>
       </c>
-      <c r="B34" s="316" t="s">
+      <c r="B34" s="361" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="317"/>
+      <c r="C34" s="362"/>
       <c r="D34" s="94">
         <v>150</v>
       </c>
@@ -5505,12 +5517,12 @@
         <v>107</v>
       </c>
       <c r="AC34" s="114"/>
-      <c r="AD34" s="341"/>
+      <c r="AD34" s="349"/>
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A35" s="310"/>
-      <c r="B35" s="318"/>
-      <c r="C35" s="319"/>
+      <c r="A35" s="381"/>
+      <c r="B35" s="365"/>
+      <c r="C35" s="366"/>
       <c r="D35" s="105">
         <v>330</v>
       </c>
@@ -5520,38 +5532,38 @@
       <c r="F35" s="107">
         <v>100</v>
       </c>
-      <c r="G35" s="311"/>
-      <c r="H35" s="312"/>
-      <c r="I35" s="313"/>
-      <c r="J35" s="320"/>
-      <c r="K35" s="321"/>
-      <c r="L35" s="321"/>
-      <c r="M35" s="322"/>
-      <c r="N35" s="320"/>
-      <c r="O35" s="321"/>
-      <c r="P35" s="322"/>
-      <c r="Q35" s="311"/>
-      <c r="R35" s="312"/>
-      <c r="S35" s="323"/>
+      <c r="G35" s="333"/>
+      <c r="H35" s="334"/>
+      <c r="I35" s="380"/>
+      <c r="J35" s="331"/>
+      <c r="K35" s="379"/>
+      <c r="L35" s="379"/>
+      <c r="M35" s="332"/>
+      <c r="N35" s="331"/>
+      <c r="O35" s="379"/>
+      <c r="P35" s="332"/>
+      <c r="Q35" s="333"/>
+      <c r="R35" s="334"/>
+      <c r="S35" s="335"/>
       <c r="T35" s="302" t="s">
         <v>117</v>
       </c>
       <c r="U35" s="115"/>
-      <c r="V35" s="320"/>
-      <c r="W35" s="322"/>
-      <c r="X35" s="320"/>
-      <c r="Y35" s="322"/>
-      <c r="Z35" s="320"/>
-      <c r="AA35" s="322"/>
-      <c r="AB35" s="320"/>
-      <c r="AC35" s="322"/>
-      <c r="AD35" s="341"/>
+      <c r="V35" s="331"/>
+      <c r="W35" s="332"/>
+      <c r="X35" s="331"/>
+      <c r="Y35" s="332"/>
+      <c r="Z35" s="331"/>
+      <c r="AA35" s="332"/>
+      <c r="AB35" s="331"/>
+      <c r="AC35" s="332"/>
+      <c r="AD35" s="349"/>
     </row>
     <row r="36" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="314" t="s">
+      <c r="B36" s="344" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="315"/>
+      <c r="C36" s="345"/>
       <c r="D36" s="20">
         <v>120</v>
       </c>
@@ -5626,47 +5638,47 @@
         <v>108</v>
       </c>
       <c r="AC36" s="89"/>
-      <c r="AD36" s="341"/>
+      <c r="AD36" s="349"/>
     </row>
     <row r="37" spans="1:30" ht="28" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="359" t="s">
+      <c r="B37" s="340" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="360"/>
-      <c r="D37" s="360"/>
-      <c r="E37" s="360"/>
-      <c r="F37" s="360"/>
-      <c r="G37" s="360"/>
-      <c r="H37" s="360"/>
-      <c r="I37" s="360"/>
-      <c r="J37" s="360"/>
-      <c r="K37" s="360"/>
-      <c r="L37" s="360"/>
-      <c r="M37" s="360"/>
-      <c r="N37" s="360"/>
-      <c r="O37" s="360"/>
-      <c r="P37" s="360"/>
-      <c r="Q37" s="360"/>
-      <c r="R37" s="360"/>
-      <c r="S37" s="360"/>
-      <c r="T37" s="360"/>
-      <c r="U37" s="360"/>
-      <c r="V37" s="360"/>
-      <c r="W37" s="360"/>
-      <c r="X37" s="360"/>
-      <c r="Y37" s="360"/>
-      <c r="Z37" s="360"/>
-      <c r="AA37" s="360"/>
-      <c r="AB37" s="360"/>
-      <c r="AC37" s="360"/>
+      <c r="C37" s="341"/>
+      <c r="D37" s="341"/>
+      <c r="E37" s="341"/>
+      <c r="F37" s="341"/>
+      <c r="G37" s="341"/>
+      <c r="H37" s="341"/>
+      <c r="I37" s="341"/>
+      <c r="J37" s="341"/>
+      <c r="K37" s="341"/>
+      <c r="L37" s="341"/>
+      <c r="M37" s="341"/>
+      <c r="N37" s="341"/>
+      <c r="O37" s="341"/>
+      <c r="P37" s="341"/>
+      <c r="Q37" s="341"/>
+      <c r="R37" s="341"/>
+      <c r="S37" s="341"/>
+      <c r="T37" s="341"/>
+      <c r="U37" s="341"/>
+      <c r="V37" s="341"/>
+      <c r="W37" s="341"/>
+      <c r="X37" s="341"/>
+      <c r="Y37" s="341"/>
+      <c r="Z37" s="341"/>
+      <c r="AA37" s="341"/>
+      <c r="AB37" s="341"/>
+      <c r="AC37" s="341"/>
       <c r="AD37" s="28"/>
     </row>
     <row r="38" spans="1:30" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A38" s="258"/>
-      <c r="B38" s="326" t="s">
+      <c r="B38" s="373" t="s">
         <v>44</v>
       </c>
-      <c r="C38" s="327"/>
+      <c r="C38" s="374"/>
       <c r="D38" s="177">
         <f>SUM(((D19-D12)/2),D12)</f>
         <v>150</v>
@@ -5750,16 +5762,16 @@
         <v>206</v>
       </c>
       <c r="AC38" s="269"/>
-      <c r="AD38" s="341" t="s">
+      <c r="AD38" s="349" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="39" spans="1:30" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="258"/>
-      <c r="B39" s="314" t="s">
+      <c r="B39" s="344" t="s">
         <v>191</v>
       </c>
-      <c r="C39" s="315"/>
+      <c r="C39" s="345"/>
       <c r="D39" s="120">
         <f>SUM(((D20-D11)/2),D11)</f>
         <v>210</v>
@@ -5843,14 +5855,14 @@
         <v>207</v>
       </c>
       <c r="AC39" s="270"/>
-      <c r="AD39" s="341"/>
+      <c r="AD39" s="349"/>
     </row>
     <row r="40" spans="1:30" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="258"/>
-      <c r="B40" s="328" t="s">
+      <c r="B40" s="375" t="s">
         <v>192</v>
       </c>
-      <c r="C40" s="329"/>
+      <c r="C40" s="376"/>
       <c r="D40" s="118">
         <f>SUM(((D21-D10)/2),D10)</f>
         <v>90</v>
@@ -5918,10 +5930,10 @@
         <v>66</v>
       </c>
       <c r="U40" s="35"/>
-      <c r="V40" s="324" t="s">
+      <c r="V40" s="377" t="s">
         <v>151</v>
       </c>
-      <c r="W40" s="325"/>
+      <c r="W40" s="378"/>
       <c r="X40" s="244" t="s">
         <v>202</v>
       </c>
@@ -5934,14 +5946,14 @@
         <v>208</v>
       </c>
       <c r="AC40" s="271"/>
-      <c r="AD40" s="341"/>
+      <c r="AD40" s="349"/>
     </row>
     <row r="41" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A41" s="231"/>
-      <c r="B41" s="316" t="s">
+      <c r="B41" s="361" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="317"/>
+      <c r="C41" s="362"/>
       <c r="D41" s="94">
         <f>SUM(((D24-D12)/2),D12)</f>
         <v>285</v>
@@ -6025,14 +6037,14 @@
         <v>136</v>
       </c>
       <c r="AC41" s="150"/>
-      <c r="AD41" s="341"/>
+      <c r="AD41" s="349"/>
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42" s="231"/>
-      <c r="B42" s="314" t="s">
+      <c r="B42" s="344" t="s">
         <v>118</v>
       </c>
-      <c r="C42" s="315"/>
+      <c r="C42" s="345"/>
       <c r="D42" s="71">
         <f>SUM(((D20-D14)/2),D14)</f>
         <v>300</v>
@@ -6117,14 +6129,14 @@
         <v>137</v>
       </c>
       <c r="AC42" s="152"/>
-      <c r="AD42" s="341"/>
+      <c r="AD42" s="349"/>
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" s="231"/>
-      <c r="B43" s="318" t="s">
+      <c r="B43" s="365" t="s">
         <v>119</v>
       </c>
-      <c r="C43" s="319"/>
+      <c r="C43" s="366"/>
       <c r="D43" s="105">
         <f>SUM(((D33-D10)/2),D10)</f>
         <v>135</v>
@@ -6208,14 +6220,14 @@
         <v>138</v>
       </c>
       <c r="AC43" s="154"/>
-      <c r="AD43" s="341"/>
+      <c r="AD43" s="349"/>
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44" s="231"/>
-      <c r="B44" s="316" t="s">
+      <c r="B44" s="361" t="s">
         <v>46</v>
       </c>
-      <c r="C44" s="317"/>
+      <c r="C44" s="362"/>
       <c r="D44" s="94">
         <f t="shared" ref="D44:I44" si="9">SUM(((D12-D28)/2),D28)</f>
         <v>195</v>
@@ -6284,10 +6296,10 @@
         <v>149</v>
       </c>
       <c r="U44" s="165"/>
-      <c r="V44" s="316" t="s">
+      <c r="V44" s="361" t="s">
         <v>151</v>
       </c>
-      <c r="W44" s="317"/>
+      <c r="W44" s="362"/>
       <c r="X44" s="116" t="s">
         <v>153</v>
       </c>
@@ -6300,14 +6312,14 @@
         <v>156</v>
       </c>
       <c r="AC44" s="174"/>
-      <c r="AD44" s="341"/>
+      <c r="AD44" s="349"/>
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A45" s="231"/>
-      <c r="B45" s="314" t="s">
+      <c r="B45" s="344" t="s">
         <v>120</v>
       </c>
-      <c r="C45" s="315"/>
+      <c r="C45" s="345"/>
       <c r="D45" s="71">
         <f>SUM(((D32-D11)/2),D11)</f>
         <v>165</v>
@@ -6392,14 +6404,14 @@
         <v>157</v>
       </c>
       <c r="AC45" s="175"/>
-      <c r="AD45" s="341"/>
+      <c r="AD45" s="349"/>
     </row>
     <row r="46" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A46" s="231"/>
-      <c r="B46" s="318" t="s">
+      <c r="B46" s="365" t="s">
         <v>121</v>
       </c>
-      <c r="C46" s="319"/>
+      <c r="C46" s="366"/>
       <c r="D46" s="105">
         <f>SUM(((D21-D13)/2),D13)</f>
         <v>180</v>
@@ -6468,10 +6480,10 @@
         <v>59</v>
       </c>
       <c r="U46" s="167"/>
-      <c r="V46" s="318" t="s">
+      <c r="V46" s="365" t="s">
         <v>151</v>
       </c>
-      <c r="W46" s="319"/>
+      <c r="W46" s="366"/>
       <c r="X46" s="118" t="s">
         <v>155</v>
       </c>
@@ -6484,14 +6496,14 @@
         <v>158</v>
       </c>
       <c r="AC46" s="176"/>
-      <c r="AD46" s="341"/>
+      <c r="AD46" s="349"/>
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A47" s="258"/>
-      <c r="B47" s="316" t="s">
+      <c r="B47" s="361" t="s">
         <v>47</v>
       </c>
-      <c r="C47" s="317"/>
+      <c r="C47" s="362"/>
       <c r="D47" s="116">
         <f>SUM(((D26-D15)/2),D15)</f>
         <v>150</v>
@@ -6576,14 +6588,14 @@
         <v>209</v>
       </c>
       <c r="AC47" s="272"/>
-      <c r="AD47" s="341"/>
+      <c r="AD47" s="349"/>
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A48" s="258"/>
-      <c r="B48" s="314" t="s">
+      <c r="B48" s="344" t="s">
         <v>193</v>
       </c>
-      <c r="C48" s="315"/>
+      <c r="C48" s="345"/>
       <c r="D48" s="120">
         <f>SUM(((D36-D14)/2),D14)</f>
         <v>210</v>
@@ -6652,10 +6664,10 @@
         <v>67</v>
       </c>
       <c r="U48" s="41"/>
-      <c r="V48" s="314" t="s">
+      <c r="V48" s="344" t="s">
         <v>151</v>
       </c>
-      <c r="W48" s="315"/>
+      <c r="W48" s="345"/>
       <c r="X48" s="120" t="s">
         <v>204</v>
       </c>
@@ -6668,14 +6680,14 @@
         <v>210</v>
       </c>
       <c r="AC48" s="273"/>
-      <c r="AD48" s="341"/>
+      <c r="AD48" s="349"/>
     </row>
     <row r="49" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A49" s="258"/>
-      <c r="B49" s="318" t="s">
+      <c r="B49" s="365" t="s">
         <v>194</v>
       </c>
-      <c r="C49" s="319"/>
+      <c r="C49" s="366"/>
       <c r="D49" s="118">
         <f>SUM(((D27-D13)/2),D13)</f>
         <v>90</v>
@@ -6760,13 +6772,13 @@
         <v>211</v>
       </c>
       <c r="AC49" s="274"/>
-      <c r="AD49" s="341"/>
+      <c r="AD49" s="349"/>
     </row>
     <row r="50" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B50" s="316" t="s">
+      <c r="B50" s="361" t="s">
         <v>48</v>
       </c>
-      <c r="C50" s="317"/>
+      <c r="C50" s="362"/>
       <c r="D50" s="94">
         <f>SUM(((D26-D12)/2),D12)</f>
         <v>240</v>
@@ -6835,10 +6847,10 @@
         <v>63</v>
       </c>
       <c r="U50" s="198"/>
-      <c r="V50" s="316" t="s">
+      <c r="V50" s="361" t="s">
         <v>151</v>
       </c>
-      <c r="W50" s="317"/>
+      <c r="W50" s="362"/>
       <c r="X50" s="116" t="s">
         <v>171</v>
       </c>
@@ -6851,13 +6863,13 @@
         <v>180</v>
       </c>
       <c r="AC50" s="221"/>
-      <c r="AD50" s="341"/>
+      <c r="AD50" s="349"/>
     </row>
     <row r="51" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B51" s="314" t="s">
+      <c r="B51" s="344" t="s">
         <v>123</v>
       </c>
-      <c r="C51" s="315"/>
+      <c r="C51" s="345"/>
       <c r="D51" s="71">
         <f>SUM(((D14-D32)/2),D32)</f>
         <v>255</v>
@@ -6926,10 +6938,10 @@
         <v>159</v>
       </c>
       <c r="U51" s="199"/>
-      <c r="V51" s="314" t="s">
+      <c r="V51" s="344" t="s">
         <v>151</v>
       </c>
-      <c r="W51" s="315"/>
+      <c r="W51" s="345"/>
       <c r="X51" s="120" t="s">
         <v>172</v>
       </c>
@@ -6942,13 +6954,13 @@
         <v>181</v>
       </c>
       <c r="AC51" s="222"/>
-      <c r="AD51" s="341"/>
+      <c r="AD51" s="349"/>
     </row>
     <row r="52" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B52" s="318" t="s">
+      <c r="B52" s="365" t="s">
         <v>124</v>
       </c>
-      <c r="C52" s="319"/>
+      <c r="C52" s="366"/>
       <c r="D52" s="105">
         <f>SUM(((D33-D13)/2),D13)</f>
         <v>225</v>
@@ -7017,10 +7029,10 @@
         <v>160</v>
       </c>
       <c r="U52" s="200"/>
-      <c r="V52" s="318" t="s">
+      <c r="V52" s="365" t="s">
         <v>151</v>
       </c>
-      <c r="W52" s="319"/>
+      <c r="W52" s="366"/>
       <c r="X52" s="118" t="s">
         <v>173</v>
       </c>
@@ -7033,13 +7045,13 @@
         <v>182</v>
       </c>
       <c r="AC52" s="223"/>
-      <c r="AD52" s="341"/>
+      <c r="AD52" s="349"/>
     </row>
     <row r="53" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B53" s="316" t="s">
+      <c r="B53" s="361" t="s">
         <v>49</v>
       </c>
-      <c r="C53" s="317"/>
+      <c r="C53" s="362"/>
       <c r="D53" s="131">
         <f>SUM(((D28-D15)/2),D15)</f>
         <v>105</v>
@@ -7124,16 +7136,16 @@
         <v>183</v>
       </c>
       <c r="AC53" s="224"/>
-      <c r="AD53" s="341"/>
+      <c r="AD53" s="349"/>
       <c r="AI53" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B54" s="314" t="s">
+      <c r="B54" s="344" t="s">
         <v>125</v>
       </c>
-      <c r="C54" s="315"/>
+      <c r="C54" s="345"/>
       <c r="D54" s="133">
         <f>SUM(((D36-D11)/2),D11)</f>
         <v>120</v>
@@ -7218,13 +7230,13 @@
         <v>184</v>
       </c>
       <c r="AC54" s="225"/>
-      <c r="AD54" s="341"/>
+      <c r="AD54" s="349"/>
     </row>
     <row r="55" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B55" s="318" t="s">
+      <c r="B55" s="365" t="s">
         <v>126</v>
       </c>
-      <c r="C55" s="319"/>
+      <c r="C55" s="366"/>
       <c r="D55" s="135">
         <f>SUM(((D13-D31)/2),D31)</f>
         <v>135</v>
@@ -7309,13 +7321,13 @@
         <v>185</v>
       </c>
       <c r="AC55" s="226"/>
-      <c r="AD55" s="341"/>
+      <c r="AD55" s="349"/>
     </row>
     <row r="56" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B56" s="316" t="s">
+      <c r="B56" s="361" t="s">
         <v>50</v>
       </c>
-      <c r="C56" s="317"/>
+      <c r="C56" s="362"/>
       <c r="D56" s="131">
         <v>15</v>
       </c>
@@ -7399,13 +7411,13 @@
         <v>186</v>
       </c>
       <c r="AC56" s="227"/>
-      <c r="AD56" s="341"/>
+      <c r="AD56" s="349"/>
     </row>
     <row r="57" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B57" s="314" t="s">
+      <c r="B57" s="344" t="s">
         <v>127</v>
       </c>
-      <c r="C57" s="315"/>
+      <c r="C57" s="345"/>
       <c r="D57" s="133">
         <v>345</v>
       </c>
@@ -7488,13 +7500,13 @@
         <v>187</v>
       </c>
       <c r="AC57" s="228"/>
-      <c r="AD57" s="341"/>
+      <c r="AD57" s="349"/>
     </row>
     <row r="58" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="342" t="s">
+      <c r="B58" s="359" t="s">
         <v>128</v>
       </c>
-      <c r="C58" s="343"/>
+      <c r="C58" s="360"/>
       <c r="D58" s="188">
         <f>SUM(((D27-D10)/2),D10)</f>
         <v>0</v>
@@ -7579,21 +7591,99 @@
         <v>188</v>
       </c>
       <c r="AC58" s="229"/>
-      <c r="AD58" s="341"/>
+      <c r="AD58" s="349"/>
     </row>
     <row r="60" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="G60" s="340" t="s">
+      <c r="G60" s="363" t="s">
         <v>122</v>
       </c>
-      <c r="H60" s="340"/>
-      <c r="I60" s="340"/>
-      <c r="J60" s="340"/>
-      <c r="K60" s="340"/>
-      <c r="L60" s="340"/>
-      <c r="M60" s="340"/>
+      <c r="H60" s="363"/>
+      <c r="I60" s="363"/>
+      <c r="J60" s="363"/>
+      <c r="K60" s="363"/>
+      <c r="L60" s="363"/>
+      <c r="M60" s="363"/>
     </row>
   </sheetData>
   <mergeCells count="94">
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B22:C23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="B29:C30"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="J30:M30"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="Q30:S30"/>
+    <mergeCell ref="B34:C35"/>
+    <mergeCell ref="V40:W40"/>
+    <mergeCell ref="V48:W48"/>
+    <mergeCell ref="Z35:AA35"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="N35:P35"/>
+    <mergeCell ref="Q35:S35"/>
+    <mergeCell ref="V35:W35"/>
+    <mergeCell ref="X35:Y35"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="G60:M60"/>
+    <mergeCell ref="AH31:AI31"/>
+    <mergeCell ref="AD38:AD58"/>
+    <mergeCell ref="V44:W44"/>
+    <mergeCell ref="V46:W46"/>
+    <mergeCell ref="V51:W51"/>
+    <mergeCell ref="V52:W52"/>
+    <mergeCell ref="AB35:AC35"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="V50:W50"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="AD19:AD36"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="V18:W18"/>
+    <mergeCell ref="X18:Y18"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="AB18:AC18"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="Z23:AA23"/>
+    <mergeCell ref="AB23:AC23"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="X30:Y30"/>
+    <mergeCell ref="Z30:AA30"/>
+    <mergeCell ref="AB30:AC30"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="V23:W23"/>
     <mergeCell ref="Q23:S23"/>
@@ -7610,84 +7700,6 @@
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="T17:AC17"/>
-    <mergeCell ref="AD19:AD36"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="T18:U18"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="X18:Y18"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="AB18:AC18"/>
-    <mergeCell ref="X23:Y23"/>
-    <mergeCell ref="Z23:AA23"/>
-    <mergeCell ref="AB23:AC23"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="X30:Y30"/>
-    <mergeCell ref="Z30:AA30"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="V50:W50"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="G60:M60"/>
-    <mergeCell ref="AH31:AI31"/>
-    <mergeCell ref="AD38:AD58"/>
-    <mergeCell ref="V44:W44"/>
-    <mergeCell ref="V46:W46"/>
-    <mergeCell ref="V51:W51"/>
-    <mergeCell ref="V52:W52"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="AB30:AC30"/>
-    <mergeCell ref="Q30:S30"/>
-    <mergeCell ref="B34:C35"/>
-    <mergeCell ref="V40:W40"/>
-    <mergeCell ref="V48:W48"/>
-    <mergeCell ref="Z35:AA35"/>
-    <mergeCell ref="AB35:AC35"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="N35:P35"/>
-    <mergeCell ref="Q35:S35"/>
-    <mergeCell ref="V35:W35"/>
-    <mergeCell ref="X35:Y35"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="B29:C30"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="J30:M30"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B22:C23"/>
-    <mergeCell ref="G23:I23"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9015,8 +9027,8 @@
       <c r="Z20" s="13"/>
       <c r="AA20" s="283"/>
       <c r="AB20" s="284"/>
-      <c r="AF20" s="330"/>
-      <c r="AG20" s="330"/>
+      <c r="AF20" s="364"/>
+      <c r="AG20" s="364"/>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A21" s="291" t="s">
@@ -11029,10 +11041,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView showRuler="0" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11042,30 +11054,30 @@
     <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:13" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:14" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="B2" s="404" t="s">
+      <c r="B2" s="328" t="s">
         <v>258</v>
       </c>
-      <c r="C2" s="345" t="s">
+      <c r="C2" s="347" t="s">
         <v>257</v>
       </c>
-      <c r="D2" s="345"/>
-      <c r="E2" s="346"/>
-      <c r="F2" s="345" t="s">
+      <c r="D2" s="347"/>
+      <c r="E2" s="348"/>
+      <c r="F2" s="347" t="s">
         <v>256</v>
       </c>
-      <c r="G2" s="345"/>
-      <c r="H2" s="345"/>
-      <c r="I2" s="346"/>
+      <c r="G2" s="347"/>
+      <c r="H2" s="347"/>
+      <c r="I2" s="348"/>
       <c r="J2" s="306" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="304" t="s">
         <v>254</v>
       </c>
@@ -11081,16 +11093,16 @@
       <c r="E3" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="F3" s="390" t="s">
+      <c r="F3" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="379" t="s">
+      <c r="G3" s="318" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="332" t="s">
+      <c r="H3" s="329" t="s">
         <v>213</v>
       </c>
-      <c r="I3" s="333"/>
+      <c r="I3" s="330"/>
       <c r="J3" s="305">
         <v>138</v>
       </c>
@@ -11098,7 +11110,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="304" t="s">
         <v>252</v>
       </c>
@@ -11114,16 +11126,16 @@
       <c r="E4" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="390" t="s">
+      <c r="F4" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="370" t="s">
+      <c r="G4" s="315" t="s">
         <v>63</v>
       </c>
-      <c r="H4" s="401" t="s">
+      <c r="H4" s="392" t="s">
         <v>213</v>
       </c>
-      <c r="I4" s="315"/>
+      <c r="I4" s="345"/>
       <c r="J4" s="305">
         <v>139</v>
       </c>
@@ -11134,7 +11146,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="304" t="s">
         <v>250</v>
       </c>
@@ -11150,16 +11162,16 @@
       <c r="E5" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="390" t="s">
+      <c r="F5" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="376" t="s">
+      <c r="G5" s="317" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="401" t="s">
+      <c r="H5" s="392" t="s">
         <v>213</v>
       </c>
-      <c r="I5" s="315"/>
+      <c r="I5" s="345"/>
       <c r="J5" s="305">
         <v>133</v>
       </c>
@@ -11170,7 +11182,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="304" t="s">
         <v>248</v>
       </c>
@@ -11183,19 +11195,19 @@
       <c r="D6" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="E6" s="403" t="s">
+      <c r="E6" s="327" t="s">
         <v>114</v>
       </c>
-      <c r="F6" s="390" t="s">
+      <c r="F6" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="G6" s="376" t="s">
+      <c r="G6" s="317" t="s">
         <v>59</v>
       </c>
-      <c r="H6" s="401" t="s">
+      <c r="H6" s="392" t="s">
         <v>213</v>
       </c>
-      <c r="I6" s="315"/>
+      <c r="I6" s="345"/>
       <c r="J6" s="305">
         <v>132</v>
       </c>
@@ -11206,7 +11218,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="304" t="s">
         <v>246</v>
       </c>
@@ -11222,16 +11234,16 @@
       <c r="E7" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="F7" s="390" t="s">
+      <c r="F7" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="G7" s="373" t="s">
+      <c r="G7" s="316" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="401" t="s">
+      <c r="H7" s="392" t="s">
         <v>213</v>
       </c>
-      <c r="I7" s="315"/>
+      <c r="I7" s="345"/>
       <c r="J7" s="305">
         <v>138</v>
       </c>
@@ -11242,7 +11254,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="304" t="s">
         <v>244</v>
       </c>
@@ -11258,21 +11270,21 @@
       <c r="E8" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="F8" s="390" t="s">
+      <c r="F8" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="369" t="s">
+      <c r="G8" s="314" t="s">
         <v>61</v>
       </c>
-      <c r="H8" s="401" t="s">
+      <c r="H8" s="392" t="s">
         <v>213</v>
       </c>
-      <c r="I8" s="315"/>
+      <c r="I8" s="345"/>
       <c r="J8" s="305">
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="304" t="s">
         <v>243</v>
       </c>
@@ -11288,24 +11300,24 @@
       <c r="E9" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="376" t="s">
+      <c r="F9" s="317" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="373" t="s">
+      <c r="G9" s="316" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="401" t="s">
+      <c r="H9" s="392" t="s">
         <v>213</v>
       </c>
-      <c r="I9" s="315"/>
+      <c r="I9" s="345"/>
       <c r="J9" s="305">
         <v>140</v>
       </c>
       <c r="L9" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="304" t="s">
         <v>242</v>
       </c>
@@ -11321,27 +11333,33 @@
       <c r="E10" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="373" t="s">
+      <c r="F10" s="316" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="369" t="s">
+      <c r="G10" s="314" t="s">
         <v>61</v>
       </c>
-      <c r="H10" s="401" t="s">
+      <c r="H10" s="392" t="s">
         <v>213</v>
       </c>
-      <c r="I10" s="315"/>
+      <c r="I10" s="345"/>
       <c r="J10" s="305">
         <v>129</v>
       </c>
-      <c r="L10" s="376" t="s">
-        <v>59</v>
-      </c>
-      <c r="M10" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K10" s="326" t="s">
+        <v>217</v>
+      </c>
+      <c r="L10" s="323" t="s">
+        <v>68</v>
+      </c>
+      <c r="M10" s="321" t="s">
+        <v>56</v>
+      </c>
+      <c r="N10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="304" t="s">
         <v>241</v>
       </c>
@@ -11357,21 +11375,21 @@
       <c r="E11" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="379" t="s">
+      <c r="F11" s="318" t="s">
         <v>70</v>
       </c>
-      <c r="G11" s="376" t="s">
+      <c r="G11" s="317" t="s">
         <v>59</v>
       </c>
-      <c r="H11" s="401" t="s">
+      <c r="H11" s="392" t="s">
         <v>213</v>
       </c>
-      <c r="I11" s="315"/>
+      <c r="I11" s="345"/>
       <c r="J11" s="305">
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="304" t="s">
         <v>240</v>
       </c>
@@ -11387,21 +11405,24 @@
       <c r="E12" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="379" t="s">
+      <c r="F12" s="318" t="s">
         <v>70</v>
       </c>
-      <c r="G12" s="373" t="s">
+      <c r="G12" s="316" t="s">
         <v>60</v>
       </c>
-      <c r="H12" s="401" t="s">
+      <c r="H12" s="392" t="s">
         <v>213</v>
       </c>
-      <c r="I12" s="315"/>
+      <c r="I12" s="345"/>
       <c r="J12" s="305">
         <v>136</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L12" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="304" t="s">
         <v>239</v>
       </c>
@@ -11417,21 +11438,27 @@
       <c r="E13" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="F13" s="379" t="s">
+      <c r="F13" s="318" t="s">
         <v>70</v>
       </c>
-      <c r="G13" s="373" t="s">
+      <c r="G13" s="316" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="401" t="s">
+      <c r="H13" s="392" t="s">
         <v>213</v>
       </c>
-      <c r="I13" s="315"/>
+      <c r="I13" s="345"/>
       <c r="J13" s="305">
         <v>130</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L13" s="317" t="s">
+        <v>59</v>
+      </c>
+      <c r="M13" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="304" t="s">
         <v>238</v>
       </c>
@@ -11447,21 +11474,21 @@
       <c r="E14" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="379" t="s">
+      <c r="F14" s="318" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="369" t="s">
+      <c r="G14" s="314" t="s">
         <v>61</v>
       </c>
-      <c r="H14" s="401" t="s">
+      <c r="H14" s="392" t="s">
         <v>213</v>
       </c>
-      <c r="I14" s="315"/>
+      <c r="I14" s="345"/>
       <c r="J14" s="305">
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="304" t="s">
         <v>237</v>
       </c>
@@ -11477,21 +11504,21 @@
       <c r="E15" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="370" t="s">
+      <c r="F15" s="315" t="s">
         <v>63</v>
       </c>
-      <c r="G15" s="376" t="s">
+      <c r="G15" s="317" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="401" t="s">
+      <c r="H15" s="392" t="s">
         <v>213</v>
       </c>
-      <c r="I15" s="315"/>
+      <c r="I15" s="345"/>
       <c r="J15" s="305">
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="304" t="s">
         <v>236</v>
       </c>
@@ -11507,16 +11534,16 @@
       <c r="E16" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="F16" s="370" t="s">
+      <c r="F16" s="315" t="s">
         <v>63</v>
       </c>
-      <c r="G16" s="373" t="s">
+      <c r="G16" s="316" t="s">
         <v>60</v>
       </c>
-      <c r="H16" s="401" t="s">
+      <c r="H16" s="392" t="s">
         <v>213</v>
       </c>
-      <c r="I16" s="315"/>
+      <c r="I16" s="345"/>
       <c r="J16" s="305">
         <v>133</v>
       </c>
@@ -11537,16 +11564,16 @@
       <c r="E17" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="F17" s="370" t="s">
+      <c r="F17" s="315" t="s">
         <v>63</v>
       </c>
-      <c r="G17" s="369" t="s">
+      <c r="G17" s="314" t="s">
         <v>61</v>
       </c>
-      <c r="H17" s="401" t="s">
+      <c r="H17" s="392" t="s">
         <v>213</v>
       </c>
-      <c r="I17" s="315"/>
+      <c r="I17" s="345"/>
       <c r="J17" s="305">
         <v>135</v>
       </c>
@@ -11564,19 +11591,19 @@
       <c r="D18" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="E18" s="402" t="s">
+      <c r="E18" s="326" t="s">
         <v>217</v>
       </c>
-      <c r="F18" s="370" t="s">
+      <c r="F18" s="315" t="s">
         <v>63</v>
       </c>
-      <c r="G18" s="369" t="s">
+      <c r="G18" s="314" t="s">
         <v>61</v>
       </c>
-      <c r="H18" s="401" t="s">
+      <c r="H18" s="392" t="s">
         <v>213</v>
       </c>
-      <c r="I18" s="315"/>
+      <c r="I18" s="345"/>
       <c r="J18" s="305">
         <v>140</v>
       </c>
@@ -11597,16 +11624,16 @@
       <c r="E19" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="376" t="s">
+      <c r="F19" s="317" t="s">
         <v>59</v>
       </c>
-      <c r="G19" s="369" t="s">
+      <c r="G19" s="314" t="s">
         <v>61</v>
       </c>
-      <c r="H19" s="401" t="s">
+      <c r="H19" s="392" t="s">
         <v>213</v>
       </c>
-      <c r="I19" s="315"/>
+      <c r="I19" s="345"/>
       <c r="J19" s="305">
         <v>130</v>
       </c>
@@ -11618,10 +11645,10 @@
       <c r="B20" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="C20" s="390" t="s">
+      <c r="C20" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="379" t="s">
+      <c r="D20" s="318" t="s">
         <v>70</v>
       </c>
       <c r="E20" s="305" t="s">
@@ -11633,10 +11660,10 @@
       <c r="G20" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H20" s="400" t="s">
+      <c r="H20" s="401" t="s">
         <v>61</v>
       </c>
-      <c r="I20" s="399"/>
+      <c r="I20" s="402"/>
       <c r="J20" s="305">
         <v>140</v>
       </c>
@@ -11648,10 +11675,10 @@
       <c r="B21" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="C21" s="390" t="s">
+      <c r="C21" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="370" t="s">
+      <c r="D21" s="315" t="s">
         <v>63</v>
       </c>
       <c r="E21" s="305" t="s">
@@ -11663,10 +11690,10 @@
       <c r="G21" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H21" s="398" t="s">
+      <c r="H21" s="403" t="s">
         <v>60</v>
       </c>
-      <c r="I21" s="397"/>
+      <c r="I21" s="404"/>
       <c r="J21" s="305">
         <v>139</v>
       </c>
@@ -11678,10 +11705,10 @@
       <c r="B22" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="C22" s="379" t="s">
+      <c r="C22" s="318" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="370" t="s">
+      <c r="D22" s="315" t="s">
         <v>63</v>
       </c>
       <c r="E22" s="305" t="s">
@@ -11693,10 +11720,10 @@
       <c r="G22" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H22" s="396" t="s">
+      <c r="H22" s="405" t="s">
         <v>59</v>
       </c>
-      <c r="I22" s="395"/>
+      <c r="I22" s="406"/>
       <c r="J22" s="305">
         <v>135</v>
       </c>
@@ -11708,10 +11735,10 @@
       <c r="B23" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="C23" s="390" t="s">
+      <c r="C23" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="376" t="s">
+      <c r="D23" s="317" t="s">
         <v>59</v>
       </c>
       <c r="E23" s="305" t="s">
@@ -11723,10 +11750,10 @@
       <c r="G23" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H23" s="394" t="s">
+      <c r="H23" s="325" t="s">
         <v>66</v>
       </c>
-      <c r="I23" s="393" t="s">
+      <c r="I23" s="324" t="s">
         <v>114</v>
       </c>
       <c r="J23" s="305">
@@ -11740,10 +11767,10 @@
       <c r="B24" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="C24" s="390" t="s">
+      <c r="C24" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="D24" s="373" t="s">
+      <c r="D24" s="316" t="s">
         <v>60</v>
       </c>
       <c r="E24" s="305" t="s">
@@ -11755,7 +11782,7 @@
       <c r="G24" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H24" s="392" t="s">
+      <c r="H24" s="390" t="s">
         <v>68</v>
       </c>
       <c r="I24" s="391"/>
@@ -11770,10 +11797,10 @@
       <c r="B25" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="C25" s="390" t="s">
+      <c r="C25" s="322" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="369" t="s">
+      <c r="D25" s="314" t="s">
         <v>61</v>
       </c>
       <c r="E25" s="305" t="s">
@@ -11785,10 +11812,10 @@
       <c r="G25" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H25" s="389" t="s">
+      <c r="H25" s="388" t="s">
         <v>69</v>
       </c>
-      <c r="I25" s="388"/>
+      <c r="I25" s="389"/>
       <c r="J25" s="305">
         <v>139</v>
       </c>
@@ -11800,10 +11827,10 @@
       <c r="B26" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="C26" s="376" t="s">
+      <c r="C26" s="317" t="s">
         <v>59</v>
       </c>
-      <c r="D26" s="373" t="s">
+      <c r="D26" s="316" t="s">
         <v>60</v>
       </c>
       <c r="E26" s="305" t="s">
@@ -11815,10 +11842,10 @@
       <c r="G26" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H26" s="387" t="s">
+      <c r="H26" s="386" t="s">
         <v>63</v>
       </c>
-      <c r="I26" s="386"/>
+      <c r="I26" s="387"/>
       <c r="J26" s="305">
         <v>139</v>
       </c>
@@ -11830,10 +11857,10 @@
       <c r="B27" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="C27" s="373" t="s">
+      <c r="C27" s="316" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="369" t="s">
+      <c r="D27" s="314" t="s">
         <v>61</v>
       </c>
       <c r="E27" s="305" t="s">
@@ -11845,10 +11872,10 @@
       <c r="G27" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H27" s="385" t="s">
+      <c r="H27" s="384" t="s">
         <v>56</v>
       </c>
-      <c r="I27" s="384"/>
+      <c r="I27" s="385"/>
       <c r="J27" s="305">
         <v>143</v>
       </c>
@@ -11860,10 +11887,10 @@
       <c r="B28" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="C28" s="379" t="s">
+      <c r="C28" s="318" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="376" t="s">
+      <c r="D28" s="317" t="s">
         <v>59</v>
       </c>
       <c r="E28" s="305" t="s">
@@ -11875,10 +11902,10 @@
       <c r="G28" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H28" s="383" t="s">
+      <c r="H28" s="382" t="s">
         <v>64</v>
       </c>
-      <c r="I28" s="382"/>
+      <c r="I28" s="383"/>
       <c r="J28" s="305">
         <v>141</v>
       </c>
@@ -11890,10 +11917,10 @@
       <c r="B29" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="C29" s="379" t="s">
+      <c r="C29" s="318" t="s">
         <v>70</v>
       </c>
-      <c r="D29" s="373" t="s">
+      <c r="D29" s="316" t="s">
         <v>60</v>
       </c>
       <c r="E29" s="305" t="s">
@@ -11905,10 +11932,10 @@
       <c r="G29" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H29" s="381" t="s">
+      <c r="H29" s="320" t="s">
         <v>67</v>
       </c>
-      <c r="I29" s="380" t="s">
+      <c r="I29" s="319" t="s">
         <v>69</v>
       </c>
       <c r="J29" s="305">
@@ -11922,10 +11949,10 @@
       <c r="B30" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="C30" s="379" t="s">
+      <c r="C30" s="318" t="s">
         <v>70</v>
       </c>
-      <c r="D30" s="369" t="s">
+      <c r="D30" s="314" t="s">
         <v>61</v>
       </c>
       <c r="E30" s="305" t="s">
@@ -11937,10 +11964,10 @@
       <c r="G30" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H30" s="378" t="s">
+      <c r="H30" s="399" t="s">
         <v>66</v>
       </c>
-      <c r="I30" s="377"/>
+      <c r="I30" s="400"/>
       <c r="J30" s="305">
         <v>146</v>
       </c>
@@ -11952,10 +11979,10 @@
       <c r="B31" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="C31" s="370" t="s">
+      <c r="C31" s="315" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="376" t="s">
+      <c r="D31" s="317" t="s">
         <v>59</v>
       </c>
       <c r="E31" s="305" t="s">
@@ -11967,10 +11994,10 @@
       <c r="G31" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H31" s="375" t="s">
+      <c r="H31" s="397" t="s">
         <v>67</v>
       </c>
-      <c r="I31" s="374"/>
+      <c r="I31" s="398"/>
       <c r="J31" s="305">
         <v>137</v>
       </c>
@@ -11982,10 +12009,10 @@
       <c r="B32" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="C32" s="370" t="s">
+      <c r="C32" s="315" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="373" t="s">
+      <c r="D32" s="316" t="s">
         <v>60</v>
       </c>
       <c r="E32" s="305" t="s">
@@ -11997,10 +12024,10 @@
       <c r="G32" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H32" s="372" t="s">
+      <c r="H32" s="395" t="s">
         <v>65</v>
       </c>
-      <c r="I32" s="371"/>
+      <c r="I32" s="396"/>
       <c r="J32" s="305">
         <v>135</v>
       </c>
@@ -12012,10 +12039,10 @@
       <c r="B33" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="C33" s="370" t="s">
+      <c r="C33" s="315" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="369" t="s">
+      <c r="D33" s="314" t="s">
         <v>61</v>
       </c>
       <c r="E33" s="305" t="s">
@@ -12027,10 +12054,10 @@
       <c r="G33" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H33" s="368" t="s">
+      <c r="H33" s="313" t="s">
         <v>64</v>
       </c>
-      <c r="I33" s="367" t="s">
+      <c r="I33" s="312" t="s">
         <v>217</v>
       </c>
       <c r="J33" s="305">
@@ -12044,10 +12071,10 @@
       <c r="B34" s="18" t="s">
         <v>215</v>
       </c>
-      <c r="C34" s="366" t="s">
+      <c r="C34" s="311" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="365" t="s">
+      <c r="D34" s="310" t="s">
         <v>61</v>
       </c>
       <c r="E34" s="308" t="s">
@@ -12059,21 +12086,31 @@
       <c r="G34" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="H34" s="364" t="s">
+      <c r="H34" s="393" t="s">
         <v>70</v>
       </c>
-      <c r="I34" s="363"/>
+      <c r="I34" s="394"/>
       <c r="J34" s="308">
         <v>138</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="H34:I34"/>
     <mergeCell ref="H32:I32"/>
@@ -12084,22 +12121,12 @@
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
     <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H24:I24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
More thesis: started question analysis.
</commit_message>
<xml_diff>
--- a/Documents/Color Mixtures/Color Blends.xlsx
+++ b/Documents/Color Mixtures/Color Blends.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="26900" windowHeight="15400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Color Mixtures First Study" sheetId="1" r:id="rId1"/>
@@ -2061,7 +2061,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="407">
+  <cellXfs count="408">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2999,71 +2999,107 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="41" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="41" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="41" borderId="37" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="41" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="41" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="41" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="41" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3089,73 +3125,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="41" borderId="37" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3188,49 +3233,7 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="116" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3628,10 +3631,10 @@
   </sheetPr>
   <dimension ref="A2:AI60"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A15" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="T1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="D34" sqref="D34"/>
+      <selection pane="topRight" activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3646,10 +3649,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B2" s="364" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="364"/>
+      <c r="B2" s="345" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="345"/>
       <c r="E2" t="s">
         <v>7</v>
       </c>
@@ -3832,10 +3835,10 @@
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B10" s="368" t="s">
+      <c r="B10" s="350" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="368"/>
+      <c r="C10" s="350"/>
       <c r="D10" s="4">
         <v>0</v>
       </c>
@@ -3890,10 +3893,10 @@
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B11" s="369" t="s">
+      <c r="B11" s="351" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="369"/>
+      <c r="C11" s="351"/>
       <c r="D11" s="4">
         <v>120</v>
       </c>
@@ -3948,10 +3951,10 @@
       </c>
     </row>
     <row r="12" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="370" t="s">
+      <c r="B12" s="352" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="370"/>
+      <c r="C12" s="352"/>
       <c r="D12" s="25">
         <v>240</v>
       </c>
@@ -4006,10 +4009,10 @@
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B13" s="371" t="s">
+      <c r="B13" s="353" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="371"/>
+      <c r="C13" s="353"/>
       <c r="D13" s="4">
         <v>180</v>
       </c>
@@ -4064,10 +4067,10 @@
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B14" s="372" t="s">
+      <c r="B14" s="354" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="372"/>
+      <c r="C14" s="354"/>
       <c r="D14" s="4">
         <v>300</v>
       </c>
@@ -4122,10 +4125,10 @@
       </c>
     </row>
     <row r="15" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="367" t="s">
+      <c r="B15" s="349" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="367"/>
+      <c r="C15" s="349"/>
       <c r="D15" s="6">
         <v>60</v>
       </c>
@@ -4181,52 +4184,52 @@
     </row>
     <row r="16" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:35" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="336" t="s">
+      <c r="B17" s="371" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="337"/>
-      <c r="D17" s="350" t="s">
+      <c r="C17" s="372"/>
+      <c r="D17" s="346" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="329"/>
-      <c r="F17" s="330"/>
-      <c r="G17" s="329" t="s">
+      <c r="E17" s="347"/>
+      <c r="F17" s="348"/>
+      <c r="G17" s="347" t="s">
         <v>9</v>
       </c>
-      <c r="H17" s="329"/>
-      <c r="I17" s="330"/>
-      <c r="J17" s="350" t="s">
+      <c r="H17" s="347"/>
+      <c r="I17" s="348"/>
+      <c r="J17" s="346" t="s">
         <v>10</v>
       </c>
-      <c r="K17" s="329"/>
-      <c r="L17" s="329"/>
-      <c r="M17" s="330"/>
-      <c r="N17" s="350" t="s">
+      <c r="K17" s="347"/>
+      <c r="L17" s="347"/>
+      <c r="M17" s="348"/>
+      <c r="N17" s="346" t="s">
         <v>27</v>
       </c>
-      <c r="O17" s="329"/>
-      <c r="P17" s="329"/>
-      <c r="Q17" s="351" t="s">
+      <c r="O17" s="347"/>
+      <c r="P17" s="347"/>
+      <c r="Q17" s="363" t="s">
         <v>91</v>
       </c>
-      <c r="R17" s="352"/>
-      <c r="S17" s="353"/>
-      <c r="T17" s="346" t="s">
+      <c r="R17" s="364"/>
+      <c r="S17" s="365"/>
+      <c r="T17" s="379" t="s">
         <v>51</v>
       </c>
-      <c r="U17" s="347"/>
-      <c r="V17" s="347"/>
-      <c r="W17" s="347"/>
-      <c r="X17" s="347"/>
-      <c r="Y17" s="347"/>
-      <c r="Z17" s="347"/>
-      <c r="AA17" s="347"/>
-      <c r="AB17" s="347"/>
-      <c r="AC17" s="348"/>
+      <c r="U17" s="380"/>
+      <c r="V17" s="380"/>
+      <c r="W17" s="380"/>
+      <c r="X17" s="380"/>
+      <c r="Y17" s="380"/>
+      <c r="Z17" s="380"/>
+      <c r="AA17" s="380"/>
+      <c r="AB17" s="380"/>
+      <c r="AC17" s="381"/>
     </row>
     <row r="18" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="338"/>
-      <c r="C18" s="339"/>
+      <c r="B18" s="373"/>
+      <c r="C18" s="374"/>
       <c r="D18" s="22" t="s">
         <v>37</v>
       </c>
@@ -4275,32 +4278,32 @@
       <c r="S18" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="T18" s="354" t="s">
+      <c r="T18" s="366" t="s">
         <v>8</v>
       </c>
-      <c r="U18" s="355"/>
-      <c r="V18" s="356" t="s">
+      <c r="U18" s="367"/>
+      <c r="V18" s="368" t="s">
         <v>92</v>
       </c>
-      <c r="W18" s="355"/>
-      <c r="X18" s="356" t="s">
+      <c r="W18" s="367"/>
+      <c r="X18" s="368" t="s">
         <v>10</v>
       </c>
-      <c r="Y18" s="355"/>
-      <c r="Z18" s="356" t="s">
+      <c r="Y18" s="367"/>
+      <c r="Z18" s="368" t="s">
         <v>27</v>
       </c>
-      <c r="AA18" s="355"/>
-      <c r="AB18" s="357" t="s">
+      <c r="AA18" s="367"/>
+      <c r="AB18" s="369" t="s">
         <v>91</v>
       </c>
-      <c r="AC18" s="358"/>
+      <c r="AC18" s="370"/>
     </row>
     <row r="19" spans="1:35" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="342" t="s">
+      <c r="B19" s="377" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="343"/>
+      <c r="C19" s="378"/>
       <c r="D19" s="20">
         <v>60</v>
       </c>
@@ -4374,15 +4377,15 @@
         <v>94</v>
       </c>
       <c r="AC19" s="75"/>
-      <c r="AD19" s="349" t="s">
+      <c r="AD19" s="356" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B20" s="342" t="s">
+      <c r="B20" s="377" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="343"/>
+      <c r="C20" s="378"/>
       <c r="D20" s="20">
         <v>300</v>
       </c>
@@ -4456,13 +4459,13 @@
         <v>95</v>
       </c>
       <c r="AC20" s="76"/>
-      <c r="AD20" s="349"/>
+      <c r="AD20" s="356"/>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B21" s="344" t="s">
+      <c r="B21" s="333" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="345"/>
+      <c r="C21" s="334"/>
       <c r="D21" s="20">
         <v>180</v>
       </c>
@@ -4537,16 +4540,16 @@
         <v>96</v>
       </c>
       <c r="AC21" s="80"/>
-      <c r="AD21" s="349"/>
+      <c r="AD21" s="356"/>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A22" s="381" t="s">
+      <c r="A22" s="329" t="s">
         <v>116</v>
       </c>
-      <c r="B22" s="361" t="s">
+      <c r="B22" s="335" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="362"/>
+      <c r="C22" s="336"/>
       <c r="D22" s="94">
         <v>90</v>
       </c>
@@ -4621,12 +4624,12 @@
         <v>97</v>
       </c>
       <c r="AC22" s="104"/>
-      <c r="AD22" s="349"/>
+      <c r="AD22" s="356"/>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A23" s="381"/>
-      <c r="B23" s="365"/>
-      <c r="C23" s="366"/>
+      <c r="A23" s="329"/>
+      <c r="B23" s="337"/>
+      <c r="C23" s="338"/>
       <c r="D23" s="105">
         <v>270</v>
       </c>
@@ -4636,38 +4639,38 @@
       <c r="F23" s="107">
         <v>100</v>
       </c>
-      <c r="G23" s="333"/>
-      <c r="H23" s="334"/>
-      <c r="I23" s="380"/>
-      <c r="J23" s="331"/>
-      <c r="K23" s="379"/>
-      <c r="L23" s="379"/>
-      <c r="M23" s="332"/>
-      <c r="N23" s="331"/>
-      <c r="O23" s="379"/>
-      <c r="P23" s="332"/>
-      <c r="Q23" s="333"/>
-      <c r="R23" s="334"/>
-      <c r="S23" s="335"/>
-      <c r="T23" s="302" t="s">
+      <c r="G23" s="330"/>
+      <c r="H23" s="331"/>
+      <c r="I23" s="332"/>
+      <c r="J23" s="339"/>
+      <c r="K23" s="340"/>
+      <c r="L23" s="340"/>
+      <c r="M23" s="341"/>
+      <c r="N23" s="339"/>
+      <c r="O23" s="340"/>
+      <c r="P23" s="341"/>
+      <c r="Q23" s="330"/>
+      <c r="R23" s="331"/>
+      <c r="S23" s="342"/>
+      <c r="T23" s="407" t="s">
         <v>114</v>
       </c>
       <c r="U23" s="109"/>
-      <c r="V23" s="331"/>
-      <c r="W23" s="332"/>
-      <c r="X23" s="331"/>
-      <c r="Y23" s="332"/>
-      <c r="Z23" s="331"/>
-      <c r="AA23" s="332"/>
-      <c r="AB23" s="331"/>
-      <c r="AC23" s="332"/>
-      <c r="AD23" s="349"/>
+      <c r="V23" s="339"/>
+      <c r="W23" s="341"/>
+      <c r="X23" s="339"/>
+      <c r="Y23" s="341"/>
+      <c r="Z23" s="339"/>
+      <c r="AA23" s="341"/>
+      <c r="AB23" s="339"/>
+      <c r="AC23" s="341"/>
+      <c r="AD23" s="356"/>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B24" s="344" t="s">
+      <c r="B24" s="333" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="345"/>
+      <c r="C24" s="334"/>
       <c r="D24" s="20">
         <v>330</v>
       </c>
@@ -4741,13 +4744,13 @@
         <v>98</v>
       </c>
       <c r="AC24" s="81"/>
-      <c r="AD24" s="349"/>
+      <c r="AD24" s="356"/>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B25" s="344" t="s">
+      <c r="B25" s="333" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="345"/>
+      <c r="C25" s="334"/>
       <c r="D25" s="20">
         <v>30</v>
       </c>
@@ -4822,13 +4825,13 @@
         <v>99</v>
       </c>
       <c r="AC25" s="82"/>
-      <c r="AD25" s="349"/>
+      <c r="AD25" s="356"/>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B26" s="344" t="s">
+      <c r="B26" s="333" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="345"/>
+      <c r="C26" s="334"/>
       <c r="D26" s="20">
         <v>240</v>
       </c>
@@ -4903,13 +4906,13 @@
         <v>100</v>
       </c>
       <c r="AC26" s="83"/>
-      <c r="AD26" s="349"/>
+      <c r="AD26" s="356"/>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B27" s="344" t="s">
+      <c r="B27" s="333" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="345"/>
+      <c r="C27" s="334"/>
       <c r="D27" s="20">
         <v>0</v>
       </c>
@@ -4983,13 +4986,13 @@
         <v>101</v>
       </c>
       <c r="AC27" s="84"/>
-      <c r="AD27" s="349"/>
+      <c r="AD27" s="356"/>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B28" s="344" t="s">
+      <c r="B28" s="333" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="345"/>
+      <c r="C28" s="334"/>
       <c r="D28" s="20">
         <v>150</v>
       </c>
@@ -5064,16 +5067,16 @@
         <v>102</v>
       </c>
       <c r="AC28" s="85"/>
-      <c r="AD28" s="349"/>
+      <c r="AD28" s="356"/>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A29" s="381" t="s">
+      <c r="A29" s="329" t="s">
         <v>116</v>
       </c>
-      <c r="B29" s="361" t="s">
+      <c r="B29" s="335" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="362"/>
+      <c r="C29" s="336"/>
       <c r="D29" s="94">
         <v>210</v>
       </c>
@@ -5147,12 +5150,12 @@
         <v>103</v>
       </c>
       <c r="AC29" s="111"/>
-      <c r="AD29" s="349"/>
+      <c r="AD29" s="356"/>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A30" s="381"/>
-      <c r="B30" s="365"/>
-      <c r="C30" s="366"/>
+      <c r="A30" s="329"/>
+      <c r="B30" s="337"/>
+      <c r="C30" s="338"/>
       <c r="D30" s="105">
         <v>30</v>
       </c>
@@ -5162,38 +5165,38 @@
       <c r="F30" s="107">
         <v>100</v>
       </c>
-      <c r="G30" s="333"/>
-      <c r="H30" s="334"/>
-      <c r="I30" s="380"/>
-      <c r="J30" s="331"/>
-      <c r="K30" s="379"/>
-      <c r="L30" s="379"/>
-      <c r="M30" s="332"/>
-      <c r="N30" s="331"/>
-      <c r="O30" s="379"/>
-      <c r="P30" s="332"/>
-      <c r="Q30" s="333"/>
-      <c r="R30" s="334"/>
-      <c r="S30" s="335"/>
+      <c r="G30" s="330"/>
+      <c r="H30" s="331"/>
+      <c r="I30" s="332"/>
+      <c r="J30" s="339"/>
+      <c r="K30" s="340"/>
+      <c r="L30" s="340"/>
+      <c r="M30" s="341"/>
+      <c r="N30" s="339"/>
+      <c r="O30" s="340"/>
+      <c r="P30" s="341"/>
+      <c r="Q30" s="330"/>
+      <c r="R30" s="331"/>
+      <c r="S30" s="342"/>
       <c r="T30" s="302" t="s">
         <v>115</v>
       </c>
       <c r="U30" s="112"/>
-      <c r="V30" s="331"/>
-      <c r="W30" s="332"/>
-      <c r="X30" s="331"/>
-      <c r="Y30" s="332"/>
-      <c r="Z30" s="331"/>
-      <c r="AA30" s="332"/>
-      <c r="AB30" s="331"/>
-      <c r="AC30" s="332"/>
-      <c r="AD30" s="349"/>
+      <c r="V30" s="339"/>
+      <c r="W30" s="341"/>
+      <c r="X30" s="339"/>
+      <c r="Y30" s="341"/>
+      <c r="Z30" s="339"/>
+      <c r="AA30" s="341"/>
+      <c r="AB30" s="339"/>
+      <c r="AC30" s="341"/>
+      <c r="AD30" s="356"/>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B31" s="344" t="s">
+      <c r="B31" s="333" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="345"/>
+      <c r="C31" s="334"/>
       <c r="D31" s="20">
         <v>90</v>
       </c>
@@ -5268,17 +5271,17 @@
         <v>104</v>
       </c>
       <c r="AC31" s="86"/>
-      <c r="AD31" s="349"/>
-      <c r="AH31" s="364" t="s">
+      <c r="AD31" s="356"/>
+      <c r="AH31" s="345" t="s">
         <v>93</v>
       </c>
-      <c r="AI31" s="364"/>
+      <c r="AI31" s="345"/>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B32" s="344" t="s">
+      <c r="B32" s="333" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="345"/>
+      <c r="C32" s="334"/>
       <c r="D32" s="20">
         <v>210</v>
       </c>
@@ -5353,13 +5356,13 @@
         <v>105</v>
       </c>
       <c r="AC32" s="87"/>
-      <c r="AD32" s="349"/>
+      <c r="AD32" s="356"/>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B33" s="344" t="s">
+      <c r="B33" s="333" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="345"/>
+      <c r="C33" s="334"/>
       <c r="D33" s="20">
         <v>270</v>
       </c>
@@ -5434,16 +5437,16 @@
         <v>106</v>
       </c>
       <c r="AC33" s="88"/>
-      <c r="AD33" s="349"/>
+      <c r="AD33" s="356"/>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A34" s="381" t="s">
+      <c r="A34" s="329" t="s">
         <v>116</v>
       </c>
-      <c r="B34" s="361" t="s">
+      <c r="B34" s="335" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="362"/>
+      <c r="C34" s="336"/>
       <c r="D34" s="94">
         <v>150</v>
       </c>
@@ -5517,12 +5520,12 @@
         <v>107</v>
       </c>
       <c r="AC34" s="114"/>
-      <c r="AD34" s="349"/>
+      <c r="AD34" s="356"/>
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A35" s="381"/>
-      <c r="B35" s="365"/>
-      <c r="C35" s="366"/>
+      <c r="A35" s="329"/>
+      <c r="B35" s="337"/>
+      <c r="C35" s="338"/>
       <c r="D35" s="105">
         <v>330</v>
       </c>
@@ -5532,38 +5535,38 @@
       <c r="F35" s="107">
         <v>100</v>
       </c>
-      <c r="G35" s="333"/>
-      <c r="H35" s="334"/>
-      <c r="I35" s="380"/>
-      <c r="J35" s="331"/>
-      <c r="K35" s="379"/>
-      <c r="L35" s="379"/>
-      <c r="M35" s="332"/>
-      <c r="N35" s="331"/>
-      <c r="O35" s="379"/>
-      <c r="P35" s="332"/>
-      <c r="Q35" s="333"/>
-      <c r="R35" s="334"/>
-      <c r="S35" s="335"/>
+      <c r="G35" s="330"/>
+      <c r="H35" s="331"/>
+      <c r="I35" s="332"/>
+      <c r="J35" s="339"/>
+      <c r="K35" s="340"/>
+      <c r="L35" s="340"/>
+      <c r="M35" s="341"/>
+      <c r="N35" s="339"/>
+      <c r="O35" s="340"/>
+      <c r="P35" s="341"/>
+      <c r="Q35" s="330"/>
+      <c r="R35" s="331"/>
+      <c r="S35" s="342"/>
       <c r="T35" s="302" t="s">
         <v>117</v>
       </c>
       <c r="U35" s="115"/>
-      <c r="V35" s="331"/>
-      <c r="W35" s="332"/>
-      <c r="X35" s="331"/>
-      <c r="Y35" s="332"/>
-      <c r="Z35" s="331"/>
-      <c r="AA35" s="332"/>
-      <c r="AB35" s="331"/>
-      <c r="AC35" s="332"/>
-      <c r="AD35" s="349"/>
+      <c r="V35" s="339"/>
+      <c r="W35" s="341"/>
+      <c r="X35" s="339"/>
+      <c r="Y35" s="341"/>
+      <c r="Z35" s="339"/>
+      <c r="AA35" s="341"/>
+      <c r="AB35" s="339"/>
+      <c r="AC35" s="341"/>
+      <c r="AD35" s="356"/>
     </row>
     <row r="36" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="344" t="s">
+      <c r="B36" s="333" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="345"/>
+      <c r="C36" s="334"/>
       <c r="D36" s="20">
         <v>120</v>
       </c>
@@ -5638,47 +5641,47 @@
         <v>108</v>
       </c>
       <c r="AC36" s="89"/>
-      <c r="AD36" s="349"/>
+      <c r="AD36" s="356"/>
     </row>
     <row r="37" spans="1:30" ht="28" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="340" t="s">
+      <c r="B37" s="375" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="341"/>
-      <c r="D37" s="341"/>
-      <c r="E37" s="341"/>
-      <c r="F37" s="341"/>
-      <c r="G37" s="341"/>
-      <c r="H37" s="341"/>
-      <c r="I37" s="341"/>
-      <c r="J37" s="341"/>
-      <c r="K37" s="341"/>
-      <c r="L37" s="341"/>
-      <c r="M37" s="341"/>
-      <c r="N37" s="341"/>
-      <c r="O37" s="341"/>
-      <c r="P37" s="341"/>
-      <c r="Q37" s="341"/>
-      <c r="R37" s="341"/>
-      <c r="S37" s="341"/>
-      <c r="T37" s="341"/>
-      <c r="U37" s="341"/>
-      <c r="V37" s="341"/>
-      <c r="W37" s="341"/>
-      <c r="X37" s="341"/>
-      <c r="Y37" s="341"/>
-      <c r="Z37" s="341"/>
-      <c r="AA37" s="341"/>
-      <c r="AB37" s="341"/>
-      <c r="AC37" s="341"/>
+      <c r="C37" s="376"/>
+      <c r="D37" s="376"/>
+      <c r="E37" s="376"/>
+      <c r="F37" s="376"/>
+      <c r="G37" s="376"/>
+      <c r="H37" s="376"/>
+      <c r="I37" s="376"/>
+      <c r="J37" s="376"/>
+      <c r="K37" s="376"/>
+      <c r="L37" s="376"/>
+      <c r="M37" s="376"/>
+      <c r="N37" s="376"/>
+      <c r="O37" s="376"/>
+      <c r="P37" s="376"/>
+      <c r="Q37" s="376"/>
+      <c r="R37" s="376"/>
+      <c r="S37" s="376"/>
+      <c r="T37" s="376"/>
+      <c r="U37" s="376"/>
+      <c r="V37" s="376"/>
+      <c r="W37" s="376"/>
+      <c r="X37" s="376"/>
+      <c r="Y37" s="376"/>
+      <c r="Z37" s="376"/>
+      <c r="AA37" s="376"/>
+      <c r="AB37" s="376"/>
+      <c r="AC37" s="376"/>
       <c r="AD37" s="28"/>
     </row>
     <row r="38" spans="1:30" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A38" s="258"/>
-      <c r="B38" s="373" t="s">
+      <c r="B38" s="359" t="s">
         <v>44</v>
       </c>
-      <c r="C38" s="374"/>
+      <c r="C38" s="360"/>
       <c r="D38" s="177">
         <f>SUM(((D19-D12)/2),D12)</f>
         <v>150</v>
@@ -5762,16 +5765,16 @@
         <v>206</v>
       </c>
       <c r="AC38" s="269"/>
-      <c r="AD38" s="349" t="s">
+      <c r="AD38" s="356" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="39" spans="1:30" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="258"/>
-      <c r="B39" s="344" t="s">
+      <c r="B39" s="333" t="s">
         <v>191</v>
       </c>
-      <c r="C39" s="345"/>
+      <c r="C39" s="334"/>
       <c r="D39" s="120">
         <f>SUM(((D20-D11)/2),D11)</f>
         <v>210</v>
@@ -5855,14 +5858,14 @@
         <v>207</v>
       </c>
       <c r="AC39" s="270"/>
-      <c r="AD39" s="349"/>
+      <c r="AD39" s="356"/>
     </row>
     <row r="40" spans="1:30" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="258"/>
-      <c r="B40" s="375" t="s">
+      <c r="B40" s="361" t="s">
         <v>192</v>
       </c>
-      <c r="C40" s="376"/>
+      <c r="C40" s="362"/>
       <c r="D40" s="118">
         <f>SUM(((D21-D10)/2),D10)</f>
         <v>90</v>
@@ -5930,10 +5933,10 @@
         <v>66</v>
       </c>
       <c r="U40" s="35"/>
-      <c r="V40" s="377" t="s">
+      <c r="V40" s="343" t="s">
         <v>151</v>
       </c>
-      <c r="W40" s="378"/>
+      <c r="W40" s="344"/>
       <c r="X40" s="244" t="s">
         <v>202</v>
       </c>
@@ -5946,14 +5949,14 @@
         <v>208</v>
       </c>
       <c r="AC40" s="271"/>
-      <c r="AD40" s="349"/>
+      <c r="AD40" s="356"/>
     </row>
     <row r="41" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A41" s="231"/>
-      <c r="B41" s="361" t="s">
+      <c r="B41" s="335" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="362"/>
+      <c r="C41" s="336"/>
       <c r="D41" s="94">
         <f>SUM(((D24-D12)/2),D12)</f>
         <v>285</v>
@@ -6037,14 +6040,14 @@
         <v>136</v>
       </c>
       <c r="AC41" s="150"/>
-      <c r="AD41" s="349"/>
+      <c r="AD41" s="356"/>
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42" s="231"/>
-      <c r="B42" s="344" t="s">
+      <c r="B42" s="333" t="s">
         <v>118</v>
       </c>
-      <c r="C42" s="345"/>
+      <c r="C42" s="334"/>
       <c r="D42" s="71">
         <f>SUM(((D20-D14)/2),D14)</f>
         <v>300</v>
@@ -6129,14 +6132,14 @@
         <v>137</v>
       </c>
       <c r="AC42" s="152"/>
-      <c r="AD42" s="349"/>
+      <c r="AD42" s="356"/>
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" s="231"/>
-      <c r="B43" s="365" t="s">
+      <c r="B43" s="337" t="s">
         <v>119</v>
       </c>
-      <c r="C43" s="366"/>
+      <c r="C43" s="338"/>
       <c r="D43" s="105">
         <f>SUM(((D33-D10)/2),D10)</f>
         <v>135</v>
@@ -6220,14 +6223,14 @@
         <v>138</v>
       </c>
       <c r="AC43" s="154"/>
-      <c r="AD43" s="349"/>
+      <c r="AD43" s="356"/>
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44" s="231"/>
-      <c r="B44" s="361" t="s">
+      <c r="B44" s="335" t="s">
         <v>46</v>
       </c>
-      <c r="C44" s="362"/>
+      <c r="C44" s="336"/>
       <c r="D44" s="94">
         <f t="shared" ref="D44:I44" si="9">SUM(((D12-D28)/2),D28)</f>
         <v>195</v>
@@ -6296,10 +6299,10 @@
         <v>149</v>
       </c>
       <c r="U44" s="165"/>
-      <c r="V44" s="361" t="s">
+      <c r="V44" s="335" t="s">
         <v>151</v>
       </c>
-      <c r="W44" s="362"/>
+      <c r="W44" s="336"/>
       <c r="X44" s="116" t="s">
         <v>153</v>
       </c>
@@ -6312,14 +6315,14 @@
         <v>156</v>
       </c>
       <c r="AC44" s="174"/>
-      <c r="AD44" s="349"/>
+      <c r="AD44" s="356"/>
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A45" s="231"/>
-      <c r="B45" s="344" t="s">
+      <c r="B45" s="333" t="s">
         <v>120</v>
       </c>
-      <c r="C45" s="345"/>
+      <c r="C45" s="334"/>
       <c r="D45" s="71">
         <f>SUM(((D32-D11)/2),D11)</f>
         <v>165</v>
@@ -6404,14 +6407,14 @@
         <v>157</v>
       </c>
       <c r="AC45" s="175"/>
-      <c r="AD45" s="349"/>
+      <c r="AD45" s="356"/>
     </row>
     <row r="46" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A46" s="231"/>
-      <c r="B46" s="365" t="s">
+      <c r="B46" s="337" t="s">
         <v>121</v>
       </c>
-      <c r="C46" s="366"/>
+      <c r="C46" s="338"/>
       <c r="D46" s="105">
         <f>SUM(((D21-D13)/2),D13)</f>
         <v>180</v>
@@ -6480,10 +6483,10 @@
         <v>59</v>
       </c>
       <c r="U46" s="167"/>
-      <c r="V46" s="365" t="s">
+      <c r="V46" s="337" t="s">
         <v>151</v>
       </c>
-      <c r="W46" s="366"/>
+      <c r="W46" s="338"/>
       <c r="X46" s="118" t="s">
         <v>155</v>
       </c>
@@ -6496,14 +6499,14 @@
         <v>158</v>
       </c>
       <c r="AC46" s="176"/>
-      <c r="AD46" s="349"/>
+      <c r="AD46" s="356"/>
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A47" s="258"/>
-      <c r="B47" s="361" t="s">
+      <c r="B47" s="335" t="s">
         <v>47</v>
       </c>
-      <c r="C47" s="362"/>
+      <c r="C47" s="336"/>
       <c r="D47" s="116">
         <f>SUM(((D26-D15)/2),D15)</f>
         <v>150</v>
@@ -6588,14 +6591,14 @@
         <v>209</v>
       </c>
       <c r="AC47" s="272"/>
-      <c r="AD47" s="349"/>
+      <c r="AD47" s="356"/>
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A48" s="258"/>
-      <c r="B48" s="344" t="s">
+      <c r="B48" s="333" t="s">
         <v>193</v>
       </c>
-      <c r="C48" s="345"/>
+      <c r="C48" s="334"/>
       <c r="D48" s="120">
         <f>SUM(((D36-D14)/2),D14)</f>
         <v>210</v>
@@ -6664,10 +6667,10 @@
         <v>67</v>
       </c>
       <c r="U48" s="41"/>
-      <c r="V48" s="344" t="s">
+      <c r="V48" s="333" t="s">
         <v>151</v>
       </c>
-      <c r="W48" s="345"/>
+      <c r="W48" s="334"/>
       <c r="X48" s="120" t="s">
         <v>204</v>
       </c>
@@ -6680,14 +6683,14 @@
         <v>210</v>
       </c>
       <c r="AC48" s="273"/>
-      <c r="AD48" s="349"/>
+      <c r="AD48" s="356"/>
     </row>
     <row r="49" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A49" s="258"/>
-      <c r="B49" s="365" t="s">
+      <c r="B49" s="337" t="s">
         <v>194</v>
       </c>
-      <c r="C49" s="366"/>
+      <c r="C49" s="338"/>
       <c r="D49" s="118">
         <f>SUM(((D27-D13)/2),D13)</f>
         <v>90</v>
@@ -6772,13 +6775,13 @@
         <v>211</v>
       </c>
       <c r="AC49" s="274"/>
-      <c r="AD49" s="349"/>
+      <c r="AD49" s="356"/>
     </row>
     <row r="50" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B50" s="361" t="s">
+      <c r="B50" s="335" t="s">
         <v>48</v>
       </c>
-      <c r="C50" s="362"/>
+      <c r="C50" s="336"/>
       <c r="D50" s="94">
         <f>SUM(((D26-D12)/2),D12)</f>
         <v>240</v>
@@ -6847,10 +6850,10 @@
         <v>63</v>
       </c>
       <c r="U50" s="198"/>
-      <c r="V50" s="361" t="s">
+      <c r="V50" s="335" t="s">
         <v>151</v>
       </c>
-      <c r="W50" s="362"/>
+      <c r="W50" s="336"/>
       <c r="X50" s="116" t="s">
         <v>171</v>
       </c>
@@ -6863,13 +6866,13 @@
         <v>180</v>
       </c>
       <c r="AC50" s="221"/>
-      <c r="AD50" s="349"/>
+      <c r="AD50" s="356"/>
     </row>
     <row r="51" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B51" s="344" t="s">
+      <c r="B51" s="333" t="s">
         <v>123</v>
       </c>
-      <c r="C51" s="345"/>
+      <c r="C51" s="334"/>
       <c r="D51" s="71">
         <f>SUM(((D14-D32)/2),D32)</f>
         <v>255</v>
@@ -6938,10 +6941,10 @@
         <v>159</v>
       </c>
       <c r="U51" s="199"/>
-      <c r="V51" s="344" t="s">
+      <c r="V51" s="333" t="s">
         <v>151</v>
       </c>
-      <c r="W51" s="345"/>
+      <c r="W51" s="334"/>
       <c r="X51" s="120" t="s">
         <v>172</v>
       </c>
@@ -6954,13 +6957,13 @@
         <v>181</v>
       </c>
       <c r="AC51" s="222"/>
-      <c r="AD51" s="349"/>
+      <c r="AD51" s="356"/>
     </row>
     <row r="52" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B52" s="365" t="s">
+      <c r="B52" s="337" t="s">
         <v>124</v>
       </c>
-      <c r="C52" s="366"/>
+      <c r="C52" s="338"/>
       <c r="D52" s="105">
         <f>SUM(((D33-D13)/2),D13)</f>
         <v>225</v>
@@ -7029,10 +7032,10 @@
         <v>160</v>
       </c>
       <c r="U52" s="200"/>
-      <c r="V52" s="365" t="s">
+      <c r="V52" s="337" t="s">
         <v>151</v>
       </c>
-      <c r="W52" s="366"/>
+      <c r="W52" s="338"/>
       <c r="X52" s="118" t="s">
         <v>173</v>
       </c>
@@ -7045,13 +7048,13 @@
         <v>182</v>
       </c>
       <c r="AC52" s="223"/>
-      <c r="AD52" s="349"/>
+      <c r="AD52" s="356"/>
     </row>
     <row r="53" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B53" s="361" t="s">
+      <c r="B53" s="335" t="s">
         <v>49</v>
       </c>
-      <c r="C53" s="362"/>
+      <c r="C53" s="336"/>
       <c r="D53" s="131">
         <f>SUM(((D28-D15)/2),D15)</f>
         <v>105</v>
@@ -7136,16 +7139,16 @@
         <v>183</v>
       </c>
       <c r="AC53" s="224"/>
-      <c r="AD53" s="349"/>
+      <c r="AD53" s="356"/>
       <c r="AI53" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B54" s="344" t="s">
+      <c r="B54" s="333" t="s">
         <v>125</v>
       </c>
-      <c r="C54" s="345"/>
+      <c r="C54" s="334"/>
       <c r="D54" s="133">
         <f>SUM(((D36-D11)/2),D11)</f>
         <v>120</v>
@@ -7230,13 +7233,13 @@
         <v>184</v>
       </c>
       <c r="AC54" s="225"/>
-      <c r="AD54" s="349"/>
+      <c r="AD54" s="356"/>
     </row>
     <row r="55" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B55" s="365" t="s">
+      <c r="B55" s="337" t="s">
         <v>126</v>
       </c>
-      <c r="C55" s="366"/>
+      <c r="C55" s="338"/>
       <c r="D55" s="135">
         <f>SUM(((D13-D31)/2),D31)</f>
         <v>135</v>
@@ -7321,13 +7324,13 @@
         <v>185</v>
       </c>
       <c r="AC55" s="226"/>
-      <c r="AD55" s="349"/>
+      <c r="AD55" s="356"/>
     </row>
     <row r="56" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B56" s="361" t="s">
+      <c r="B56" s="335" t="s">
         <v>50</v>
       </c>
-      <c r="C56" s="362"/>
+      <c r="C56" s="336"/>
       <c r="D56" s="131">
         <v>15</v>
       </c>
@@ -7411,13 +7414,13 @@
         <v>186</v>
       </c>
       <c r="AC56" s="227"/>
-      <c r="AD56" s="349"/>
+      <c r="AD56" s="356"/>
     </row>
     <row r="57" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B57" s="344" t="s">
+      <c r="B57" s="333" t="s">
         <v>127</v>
       </c>
-      <c r="C57" s="345"/>
+      <c r="C57" s="334"/>
       <c r="D57" s="133">
         <v>345</v>
       </c>
@@ -7500,13 +7503,13 @@
         <v>187</v>
       </c>
       <c r="AC57" s="228"/>
-      <c r="AD57" s="349"/>
+      <c r="AD57" s="356"/>
     </row>
     <row r="58" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="359" t="s">
+      <c r="B58" s="357" t="s">
         <v>128</v>
       </c>
-      <c r="C58" s="360"/>
+      <c r="C58" s="358"/>
       <c r="D58" s="188">
         <f>SUM(((D27-D10)/2),D10)</f>
         <v>0</v>
@@ -7591,67 +7594,48 @@
         <v>188</v>
       </c>
       <c r="AC58" s="229"/>
-      <c r="AD58" s="349"/>
+      <c r="AD58" s="356"/>
     </row>
     <row r="60" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="G60" s="363" t="s">
+      <c r="G60" s="355" t="s">
         <v>122</v>
       </c>
-      <c r="H60" s="363"/>
-      <c r="I60" s="363"/>
-      <c r="J60" s="363"/>
-      <c r="K60" s="363"/>
-      <c r="L60" s="363"/>
-      <c r="M60" s="363"/>
+      <c r="H60" s="355"/>
+      <c r="I60" s="355"/>
+      <c r="J60" s="355"/>
+      <c r="K60" s="355"/>
+      <c r="L60" s="355"/>
+      <c r="M60" s="355"/>
     </row>
   </sheetData>
   <mergeCells count="94">
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B22:C23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="B29:C30"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="J30:M30"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="Q30:S30"/>
-    <mergeCell ref="B34:C35"/>
-    <mergeCell ref="V40:W40"/>
-    <mergeCell ref="V48:W48"/>
-    <mergeCell ref="Z35:AA35"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="N35:P35"/>
-    <mergeCell ref="Q35:S35"/>
-    <mergeCell ref="V35:W35"/>
-    <mergeCell ref="X35:Y35"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="G60:M60"/>
-    <mergeCell ref="AH31:AI31"/>
-    <mergeCell ref="AD38:AD58"/>
-    <mergeCell ref="V44:W44"/>
-    <mergeCell ref="V46:W46"/>
-    <mergeCell ref="V51:W51"/>
-    <mergeCell ref="V52:W52"/>
-    <mergeCell ref="AB35:AC35"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="B37:AC37"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="T17:AC17"/>
+    <mergeCell ref="X18:Y18"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="AB18:AC18"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="Z23:AA23"/>
+    <mergeCell ref="AB23:AC23"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="V18:W18"/>
     <mergeCell ref="B58:C58"/>
     <mergeCell ref="V50:W50"/>
     <mergeCell ref="B54:C54"/>
@@ -7668,38 +7652,57 @@
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="B49:C49"/>
+    <mergeCell ref="G60:M60"/>
+    <mergeCell ref="AH31:AI31"/>
+    <mergeCell ref="AD38:AD58"/>
+    <mergeCell ref="V44:W44"/>
+    <mergeCell ref="V46:W46"/>
+    <mergeCell ref="V51:W51"/>
+    <mergeCell ref="V52:W52"/>
+    <mergeCell ref="AB35:AC35"/>
     <mergeCell ref="AD19:AD36"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="T18:U18"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="X18:Y18"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="AB18:AC18"/>
-    <mergeCell ref="X23:Y23"/>
-    <mergeCell ref="Z23:AA23"/>
-    <mergeCell ref="AB23:AC23"/>
     <mergeCell ref="V30:W30"/>
     <mergeCell ref="X30:Y30"/>
     <mergeCell ref="Z30:AA30"/>
     <mergeCell ref="AB30:AC30"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="Q23:S23"/>
-    <mergeCell ref="B17:C18"/>
-    <mergeCell ref="B37:AC37"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="T17:AC17"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="Q30:S30"/>
+    <mergeCell ref="B34:C35"/>
+    <mergeCell ref="V40:W40"/>
+    <mergeCell ref="V48:W48"/>
+    <mergeCell ref="Z35:AA35"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="N35:P35"/>
+    <mergeCell ref="Q35:S35"/>
+    <mergeCell ref="V35:W35"/>
+    <mergeCell ref="X35:Y35"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="B29:C30"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="J30:M30"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B22:C23"/>
+    <mergeCell ref="G23:I23"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9027,8 +9030,8 @@
       <c r="Z20" s="13"/>
       <c r="AA20" s="283"/>
       <c r="AB20" s="284"/>
-      <c r="AF20" s="364"/>
-      <c r="AG20" s="364"/>
+      <c r="AF20" s="345"/>
+      <c r="AG20" s="345"/>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A21" s="291" t="s">
@@ -11062,17 +11065,17 @@
       <c r="B2" s="328" t="s">
         <v>258</v>
       </c>
-      <c r="C2" s="347" t="s">
+      <c r="C2" s="380" t="s">
         <v>257</v>
       </c>
-      <c r="D2" s="347"/>
-      <c r="E2" s="348"/>
-      <c r="F2" s="347" t="s">
+      <c r="D2" s="380"/>
+      <c r="E2" s="381"/>
+      <c r="F2" s="380" t="s">
         <v>256</v>
       </c>
-      <c r="G2" s="347"/>
-      <c r="H2" s="347"/>
-      <c r="I2" s="348"/>
+      <c r="G2" s="380"/>
+      <c r="H2" s="380"/>
+      <c r="I2" s="381"/>
       <c r="J2" s="306" t="s">
         <v>255</v>
       </c>
@@ -11099,10 +11102,10 @@
       <c r="G3" s="318" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="329" t="s">
+      <c r="H3" s="347" t="s">
         <v>213</v>
       </c>
-      <c r="I3" s="330"/>
+      <c r="I3" s="348"/>
       <c r="J3" s="305">
         <v>138</v>
       </c>
@@ -11132,10 +11135,10 @@
       <c r="G4" s="315" t="s">
         <v>63</v>
       </c>
-      <c r="H4" s="392" t="s">
+      <c r="H4" s="382" t="s">
         <v>213</v>
       </c>
-      <c r="I4" s="345"/>
+      <c r="I4" s="334"/>
       <c r="J4" s="305">
         <v>139</v>
       </c>
@@ -11168,10 +11171,10 @@
       <c r="G5" s="317" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="392" t="s">
+      <c r="H5" s="382" t="s">
         <v>213</v>
       </c>
-      <c r="I5" s="345"/>
+      <c r="I5" s="334"/>
       <c r="J5" s="305">
         <v>133</v>
       </c>
@@ -11204,10 +11207,10 @@
       <c r="G6" s="317" t="s">
         <v>59</v>
       </c>
-      <c r="H6" s="392" t="s">
+      <c r="H6" s="382" t="s">
         <v>213</v>
       </c>
-      <c r="I6" s="345"/>
+      <c r="I6" s="334"/>
       <c r="J6" s="305">
         <v>132</v>
       </c>
@@ -11240,10 +11243,10 @@
       <c r="G7" s="316" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="392" t="s">
+      <c r="H7" s="382" t="s">
         <v>213</v>
       </c>
-      <c r="I7" s="345"/>
+      <c r="I7" s="334"/>
       <c r="J7" s="305">
         <v>138</v>
       </c>
@@ -11276,10 +11279,10 @@
       <c r="G8" s="314" t="s">
         <v>61</v>
       </c>
-      <c r="H8" s="392" t="s">
+      <c r="H8" s="382" t="s">
         <v>213</v>
       </c>
-      <c r="I8" s="345"/>
+      <c r="I8" s="334"/>
       <c r="J8" s="305">
         <v>128</v>
       </c>
@@ -11306,10 +11309,10 @@
       <c r="G9" s="316" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="392" t="s">
+      <c r="H9" s="382" t="s">
         <v>213</v>
       </c>
-      <c r="I9" s="345"/>
+      <c r="I9" s="334"/>
       <c r="J9" s="305">
         <v>140</v>
       </c>
@@ -11339,10 +11342,10 @@
       <c r="G10" s="314" t="s">
         <v>61</v>
       </c>
-      <c r="H10" s="392" t="s">
+      <c r="H10" s="382" t="s">
         <v>213</v>
       </c>
-      <c r="I10" s="345"/>
+      <c r="I10" s="334"/>
       <c r="J10" s="305">
         <v>129</v>
       </c>
@@ -11381,10 +11384,10 @@
       <c r="G11" s="317" t="s">
         <v>59</v>
       </c>
-      <c r="H11" s="392" t="s">
+      <c r="H11" s="382" t="s">
         <v>213</v>
       </c>
-      <c r="I11" s="345"/>
+      <c r="I11" s="334"/>
       <c r="J11" s="305">
         <v>136</v>
       </c>
@@ -11411,10 +11414,10 @@
       <c r="G12" s="316" t="s">
         <v>60</v>
       </c>
-      <c r="H12" s="392" t="s">
+      <c r="H12" s="382" t="s">
         <v>213</v>
       </c>
-      <c r="I12" s="345"/>
+      <c r="I12" s="334"/>
       <c r="J12" s="305">
         <v>136</v>
       </c>
@@ -11444,10 +11447,10 @@
       <c r="G13" s="316" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="392" t="s">
+      <c r="H13" s="382" t="s">
         <v>213</v>
       </c>
-      <c r="I13" s="345"/>
+      <c r="I13" s="334"/>
       <c r="J13" s="305">
         <v>130</v>
       </c>
@@ -11480,10 +11483,10 @@
       <c r="G14" s="314" t="s">
         <v>61</v>
       </c>
-      <c r="H14" s="392" t="s">
+      <c r="H14" s="382" t="s">
         <v>213</v>
       </c>
-      <c r="I14" s="345"/>
+      <c r="I14" s="334"/>
       <c r="J14" s="305">
         <v>122</v>
       </c>
@@ -11510,10 +11513,10 @@
       <c r="G15" s="317" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="392" t="s">
+      <c r="H15" s="382" t="s">
         <v>213</v>
       </c>
-      <c r="I15" s="345"/>
+      <c r="I15" s="334"/>
       <c r="J15" s="305">
         <v>135</v>
       </c>
@@ -11540,10 +11543,10 @@
       <c r="G16" s="316" t="s">
         <v>60</v>
       </c>
-      <c r="H16" s="392" t="s">
+      <c r="H16" s="382" t="s">
         <v>213</v>
       </c>
-      <c r="I16" s="345"/>
+      <c r="I16" s="334"/>
       <c r="J16" s="305">
         <v>133</v>
       </c>
@@ -11570,10 +11573,10 @@
       <c r="G17" s="314" t="s">
         <v>61</v>
       </c>
-      <c r="H17" s="392" t="s">
+      <c r="H17" s="382" t="s">
         <v>213</v>
       </c>
-      <c r="I17" s="345"/>
+      <c r="I17" s="334"/>
       <c r="J17" s="305">
         <v>135</v>
       </c>
@@ -11600,10 +11603,10 @@
       <c r="G18" s="314" t="s">
         <v>61</v>
       </c>
-      <c r="H18" s="392" t="s">
+      <c r="H18" s="382" t="s">
         <v>213</v>
       </c>
-      <c r="I18" s="345"/>
+      <c r="I18" s="334"/>
       <c r="J18" s="305">
         <v>140</v>
       </c>
@@ -11630,10 +11633,10 @@
       <c r="G19" s="314" t="s">
         <v>61</v>
       </c>
-      <c r="H19" s="392" t="s">
+      <c r="H19" s="382" t="s">
         <v>213</v>
       </c>
-      <c r="I19" s="345"/>
+      <c r="I19" s="334"/>
       <c r="J19" s="305">
         <v>130</v>
       </c>
@@ -11660,10 +11663,10 @@
       <c r="G20" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H20" s="401" t="s">
+      <c r="H20" s="391" t="s">
         <v>61</v>
       </c>
-      <c r="I20" s="402"/>
+      <c r="I20" s="392"/>
       <c r="J20" s="305">
         <v>140</v>
       </c>
@@ -11690,10 +11693,10 @@
       <c r="G21" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H21" s="403" t="s">
+      <c r="H21" s="393" t="s">
         <v>60</v>
       </c>
-      <c r="I21" s="404"/>
+      <c r="I21" s="394"/>
       <c r="J21" s="305">
         <v>139</v>
       </c>
@@ -11720,10 +11723,10 @@
       <c r="G22" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H22" s="405" t="s">
+      <c r="H22" s="395" t="s">
         <v>59</v>
       </c>
-      <c r="I22" s="406"/>
+      <c r="I22" s="396"/>
       <c r="J22" s="305">
         <v>135</v>
       </c>
@@ -11782,10 +11785,10 @@
       <c r="G24" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H24" s="390" t="s">
+      <c r="H24" s="405" t="s">
         <v>68</v>
       </c>
-      <c r="I24" s="391"/>
+      <c r="I24" s="406"/>
       <c r="J24" s="305">
         <v>136</v>
       </c>
@@ -11812,10 +11815,10 @@
       <c r="G25" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H25" s="388" t="s">
+      <c r="H25" s="403" t="s">
         <v>69</v>
       </c>
-      <c r="I25" s="389"/>
+      <c r="I25" s="404"/>
       <c r="J25" s="305">
         <v>139</v>
       </c>
@@ -11842,10 +11845,10 @@
       <c r="G26" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H26" s="386" t="s">
+      <c r="H26" s="401" t="s">
         <v>63</v>
       </c>
-      <c r="I26" s="387"/>
+      <c r="I26" s="402"/>
       <c r="J26" s="305">
         <v>139</v>
       </c>
@@ -11872,10 +11875,10 @@
       <c r="G27" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H27" s="384" t="s">
+      <c r="H27" s="399" t="s">
         <v>56</v>
       </c>
-      <c r="I27" s="385"/>
+      <c r="I27" s="400"/>
       <c r="J27" s="305">
         <v>143</v>
       </c>
@@ -11902,10 +11905,10 @@
       <c r="G28" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H28" s="382" t="s">
+      <c r="H28" s="397" t="s">
         <v>64</v>
       </c>
-      <c r="I28" s="383"/>
+      <c r="I28" s="398"/>
       <c r="J28" s="305">
         <v>141</v>
       </c>
@@ -11964,10 +11967,10 @@
       <c r="G30" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H30" s="399" t="s">
+      <c r="H30" s="389" t="s">
         <v>66</v>
       </c>
-      <c r="I30" s="400"/>
+      <c r="I30" s="390"/>
       <c r="J30" s="305">
         <v>146</v>
       </c>
@@ -11994,10 +11997,10 @@
       <c r="G31" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H31" s="397" t="s">
+      <c r="H31" s="387" t="s">
         <v>67</v>
       </c>
-      <c r="I31" s="398"/>
+      <c r="I31" s="388"/>
       <c r="J31" s="305">
         <v>137</v>
       </c>
@@ -12024,10 +12027,10 @@
       <c r="G32" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H32" s="395" t="s">
+      <c r="H32" s="385" t="s">
         <v>65</v>
       </c>
-      <c r="I32" s="396"/>
+      <c r="I32" s="386"/>
       <c r="J32" s="305">
         <v>135</v>
       </c>
@@ -12086,31 +12089,16 @@
       <c r="G34" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="H34" s="393" t="s">
+      <c r="H34" s="383" t="s">
         <v>70</v>
       </c>
-      <c r="I34" s="394"/>
+      <c r="I34" s="384"/>
       <c r="J34" s="308">
         <v>138</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="H34:I34"/>
     <mergeCell ref="H32:I32"/>
@@ -12127,6 +12115,21 @@
     <mergeCell ref="H26:I26"/>
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>